<commit_message>
State sources and data for 5 more states ending in Ohio.
</commit_message>
<xml_diff>
--- a/data/raw/State_Sources.xlsx
+++ b/data/raw/State_Sources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chigham\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chigham\Documents\forkranger-us-regions\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECE7C1D-0511-4A66-B7F4-223B5FD810AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963C7F03-68E1-4DE3-9FA7-2B0BE110835C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="20" activeTab="28" xr2:uid="{1A035CB0-260D-4ABF-9F3B-5033D39FF1A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="26" activeTab="35" xr2:uid="{1A035CB0-260D-4ABF-9F3B-5033D39FF1A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Alabama" sheetId="1" r:id="rId1"/>
@@ -44,6 +44,11 @@
     <sheet name="Nevada" sheetId="29" r:id="rId29"/>
     <sheet name="New Hampshire" sheetId="30" r:id="rId30"/>
     <sheet name="New Jersey" sheetId="31" r:id="rId31"/>
+    <sheet name="New Mexico" sheetId="32" r:id="rId32"/>
+    <sheet name="New York" sheetId="33" r:id="rId33"/>
+    <sheet name="North Carolina" sheetId="34" r:id="rId34"/>
+    <sheet name="North Dakota" sheetId="35" r:id="rId35"/>
+    <sheet name="Ohio" sheetId="36" r:id="rId36"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6755" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8061" uniqueCount="351">
   <si>
     <t>Greens (Collards, turnips, etc.)</t>
   </si>
@@ -1059,6 +1064,66 @@
   </si>
   <si>
     <t>Tat Sol</t>
+  </si>
+  <si>
+    <t>Jalapeno</t>
+  </si>
+  <si>
+    <t>Poblano</t>
+  </si>
+  <si>
+    <t>Serrano</t>
+  </si>
+  <si>
+    <t>Roma Tomatoes</t>
+  </si>
+  <si>
+    <t>Beans, Dry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beans, Lima </t>
+  </si>
+  <si>
+    <t>Beans, Snap</t>
+  </si>
+  <si>
+    <t>Great From Storage</t>
+  </si>
+  <si>
+    <t>Bokchoy</t>
+  </si>
+  <si>
+    <t>Butterbeans</t>
+  </si>
+  <si>
+    <t>Honeydew Melons</t>
+  </si>
+  <si>
+    <t>Indian Corn</t>
+  </si>
+  <si>
+    <t>Muscadine Grapes</t>
+  </si>
+  <si>
+    <t>Romain Lettuce</t>
+  </si>
+  <si>
+    <t>Snow Peas</t>
+  </si>
+  <si>
+    <t>Snow Pea Tips</t>
+  </si>
+  <si>
+    <t>Sprite Melons</t>
+  </si>
+  <si>
+    <t>Chockcherries</t>
+  </si>
+  <si>
+    <t>Juneberries</t>
+  </si>
+  <si>
+    <t>Meskmelon</t>
   </si>
 </sst>
 </file>
@@ -15389,7 +15454,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15904,7 +15969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DAFC44-1A10-4024-A680-2AC93E634426}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A49" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -18193,10 +18258,11 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC35D6E2-8F57-4BB0-911D-C59455EE4CCA}">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:M2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18244,7 +18310,7 @@
         <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I2" t="s">
         <v>239</v>
@@ -18259,247 +18325,4659 @@
         <v>239</v>
       </c>
       <c r="M2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
+      <c r="H3" t="s">
+        <v>238</v>
+      </c>
+      <c r="I3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
+      <c r="G4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H4" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
+      <c r="G5" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>268</v>
       </c>
+      <c r="J6" t="s">
+        <v>238</v>
+      </c>
+      <c r="K6" t="s">
+        <v>239</v>
+      </c>
+      <c r="L6" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>123</v>
       </c>
+      <c r="I7" t="s">
+        <v>238</v>
+      </c>
+      <c r="J7" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
+      <c r="H8" t="s">
+        <v>238</v>
+      </c>
+      <c r="I8" t="s">
+        <v>239</v>
+      </c>
+      <c r="J8" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>168</v>
       </c>
+      <c r="H9" t="s">
+        <v>238</v>
+      </c>
+      <c r="I9" t="s">
+        <v>239</v>
+      </c>
+      <c r="J9" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>64</v>
       </c>
+      <c r="I10" t="s">
+        <v>238</v>
+      </c>
+      <c r="J10" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>65</v>
       </c>
+      <c r="H11" t="s">
+        <v>238</v>
+      </c>
+      <c r="I11" t="s">
+        <v>239</v>
+      </c>
+      <c r="J11" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
+      <c r="F12" t="s">
+        <v>238</v>
+      </c>
+      <c r="G12" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>70</v>
       </c>
+      <c r="E13" t="s">
+        <v>238</v>
+      </c>
+      <c r="F13" t="s">
+        <v>239</v>
+      </c>
+      <c r="G13" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>71</v>
       </c>
+      <c r="E14" t="s">
+        <v>238</v>
+      </c>
+      <c r="F14" t="s">
+        <v>239</v>
+      </c>
+      <c r="G14" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>36</v>
       </c>
+      <c r="G15" t="s">
+        <v>238</v>
+      </c>
+      <c r="H15" t="s">
+        <v>239</v>
+      </c>
+      <c r="I15" t="s">
+        <v>239</v>
+      </c>
+      <c r="J15" t="s">
+        <v>239</v>
+      </c>
+      <c r="K15" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" t="s">
+        <v>238</v>
+      </c>
+      <c r="H16" t="s">
+        <v>239</v>
+      </c>
+      <c r="I16" t="s">
+        <v>239</v>
+      </c>
+      <c r="J16" t="s">
+        <v>239</v>
+      </c>
+      <c r="K16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>238</v>
+      </c>
+      <c r="H17" t="s">
+        <v>239</v>
+      </c>
+      <c r="I17" t="s">
+        <v>239</v>
+      </c>
+      <c r="J17" t="s">
+        <v>239</v>
+      </c>
+      <c r="K17" t="s">
+        <v>239</v>
+      </c>
+      <c r="L17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>238</v>
+      </c>
+      <c r="F18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G18" t="s">
+        <v>237</v>
+      </c>
+      <c r="J18" t="s">
+        <v>238</v>
+      </c>
+      <c r="K18" t="s">
+        <v>239</v>
+      </c>
+      <c r="L18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" t="s">
+        <v>239</v>
+      </c>
+      <c r="K19" t="s">
+        <v>238</v>
+      </c>
+      <c r="L19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>238</v>
+      </c>
+      <c r="H20" t="s">
+        <v>239</v>
+      </c>
+      <c r="I20" t="s">
+        <v>239</v>
+      </c>
+      <c r="J20" t="s">
+        <v>239</v>
+      </c>
+      <c r="K20" t="s">
+        <v>239</v>
+      </c>
+      <c r="L20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" t="s">
+        <v>238</v>
+      </c>
+      <c r="H21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I21" t="s">
+        <v>239</v>
+      </c>
+      <c r="J21" t="s">
+        <v>239</v>
+      </c>
+      <c r="K21" t="s">
+        <v>239</v>
+      </c>
+      <c r="L21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" t="s">
+        <v>238</v>
+      </c>
+      <c r="K22" t="s">
+        <v>239</v>
+      </c>
+      <c r="L22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" t="s">
+        <v>238</v>
+      </c>
+      <c r="G23" t="s">
+        <v>239</v>
+      </c>
+      <c r="H23" t="s">
+        <v>239</v>
+      </c>
+      <c r="I23" t="s">
+        <v>239</v>
+      </c>
+      <c r="J23" t="s">
+        <v>239</v>
+      </c>
+      <c r="K23" t="s">
+        <v>239</v>
+      </c>
+      <c r="L23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>211</v>
+      </c>
+      <c r="F24" t="s">
+        <v>238</v>
+      </c>
+      <c r="G24" t="s">
+        <v>237</v>
+      </c>
+      <c r="J24" t="s">
+        <v>238</v>
+      </c>
+      <c r="K24" t="s">
+        <v>239</v>
+      </c>
+      <c r="L24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" t="s">
+        <v>238</v>
+      </c>
+      <c r="G25" t="s">
+        <v>239</v>
+      </c>
+      <c r="H25" t="s">
+        <v>239</v>
+      </c>
+      <c r="I25" t="s">
+        <v>239</v>
+      </c>
+      <c r="J25" t="s">
+        <v>239</v>
+      </c>
+      <c r="K25" t="s">
+        <v>239</v>
+      </c>
+      <c r="L25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" t="s">
+        <v>238</v>
+      </c>
+      <c r="H26" t="s">
+        <v>239</v>
+      </c>
+      <c r="I26" t="s">
+        <v>239</v>
+      </c>
+      <c r="J26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>328</v>
+      </c>
+      <c r="E27" t="s">
+        <v>238</v>
+      </c>
+      <c r="F27" t="s">
+        <v>239</v>
+      </c>
+      <c r="G27" t="s">
+        <v>237</v>
+      </c>
+      <c r="J27" t="s">
+        <v>238</v>
+      </c>
+      <c r="K27" t="s">
+        <v>239</v>
+      </c>
+      <c r="L27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" t="s">
+        <v>238</v>
+      </c>
+      <c r="I28" t="s">
+        <v>239</v>
+      </c>
+      <c r="J28" t="s">
+        <v>239</v>
+      </c>
+      <c r="K28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>137</v>
+      </c>
+      <c r="H29" t="s">
+        <v>238</v>
+      </c>
+      <c r="I29" t="s">
+        <v>239</v>
+      </c>
+      <c r="J29" t="s">
+        <v>239</v>
+      </c>
+      <c r="K29" t="s">
+        <v>239</v>
+      </c>
+      <c r="L29" t="s">
+        <v>239</v>
+      </c>
+      <c r="M29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>329</v>
+      </c>
+      <c r="F30" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>238</v>
+      </c>
+      <c r="H31" t="s">
+        <v>239</v>
+      </c>
+      <c r="I31" t="s">
+        <v>239</v>
+      </c>
+      <c r="J31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>238</v>
+      </c>
+      <c r="F32" t="s">
+        <v>239</v>
+      </c>
+      <c r="G32" t="s">
+        <v>237</v>
+      </c>
+      <c r="J32" t="s">
+        <v>238</v>
+      </c>
+      <c r="K32" t="s">
+        <v>239</v>
+      </c>
+      <c r="L32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>238</v>
+      </c>
+      <c r="F33" t="s">
+        <v>237</v>
+      </c>
+      <c r="K33" t="s">
+        <v>238</v>
+      </c>
+      <c r="L33" t="s">
+        <v>239</v>
+      </c>
+      <c r="M33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>238</v>
+      </c>
+      <c r="F34" t="s">
+        <v>239</v>
+      </c>
+      <c r="G34" t="s">
+        <v>237</v>
+      </c>
+      <c r="J34" t="s">
+        <v>238</v>
+      </c>
+      <c r="K34" t="s">
+        <v>239</v>
+      </c>
+      <c r="L34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>197</v>
+      </c>
+      <c r="H35" t="s">
+        <v>238</v>
+      </c>
+      <c r="I35" t="s">
+        <v>239</v>
+      </c>
+      <c r="J35" t="s">
+        <v>239</v>
+      </c>
+      <c r="K35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>316</v>
+      </c>
+      <c r="E36" t="s">
+        <v>238</v>
+      </c>
+      <c r="F36" t="s">
+        <v>239</v>
+      </c>
+      <c r="G36" t="s">
+        <v>237</v>
+      </c>
+      <c r="J36" t="s">
+        <v>238</v>
+      </c>
+      <c r="K36" t="s">
+        <v>239</v>
+      </c>
+      <c r="L36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="H37" t="s">
+        <v>238</v>
+      </c>
+      <c r="I37" t="s">
+        <v>239</v>
+      </c>
+      <c r="J37" t="s">
+        <v>239</v>
+      </c>
+      <c r="K37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" t="s">
+        <v>238</v>
+      </c>
+      <c r="H38" t="s">
+        <v>239</v>
+      </c>
+      <c r="I38" t="s">
+        <v>239</v>
+      </c>
+      <c r="J38" t="s">
+        <v>239</v>
+      </c>
+      <c r="K38" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="J39" t="s">
+        <v>238</v>
+      </c>
+      <c r="K39" t="s">
+        <v>239</v>
+      </c>
+      <c r="L39" t="s">
+        <v>239</v>
+      </c>
+      <c r="M39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" t="s">
+        <v>238</v>
+      </c>
+      <c r="G40" t="s">
+        <v>239</v>
+      </c>
+      <c r="H40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>158</v>
+      </c>
+      <c r="H41" t="s">
+        <v>238</v>
+      </c>
+      <c r="I41" t="s">
+        <v>239</v>
+      </c>
+      <c r="J41" t="s">
+        <v>239</v>
+      </c>
+      <c r="K41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>331</v>
+      </c>
+      <c r="H42" t="s">
+        <v>238</v>
+      </c>
+      <c r="I42" t="s">
+        <v>239</v>
+      </c>
+      <c r="J42" t="s">
+        <v>239</v>
+      </c>
+      <c r="K42" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>332</v>
+      </c>
+      <c r="H43" t="s">
+        <v>238</v>
+      </c>
+      <c r="I43" t="s">
+        <v>239</v>
+      </c>
+      <c r="J43" t="s">
+        <v>239</v>
+      </c>
+      <c r="K43" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>333</v>
+      </c>
+      <c r="H44" t="s">
+        <v>238</v>
+      </c>
+      <c r="I44" t="s">
+        <v>239</v>
+      </c>
+      <c r="J44" t="s">
+        <v>239</v>
+      </c>
+      <c r="K44" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" t="s">
+        <v>238</v>
+      </c>
+      <c r="I45" t="s">
+        <v>239</v>
+      </c>
+      <c r="J45" t="s">
+        <v>239</v>
+      </c>
+      <c r="K45" t="s">
+        <v>239</v>
+      </c>
+      <c r="L45" t="s">
+        <v>239</v>
+      </c>
+      <c r="M45" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="J46" t="s">
+        <v>238</v>
+      </c>
+      <c r="K46" t="s">
+        <v>239</v>
+      </c>
+      <c r="L46" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>116</v>
+      </c>
+      <c r="G47" t="s">
+        <v>239</v>
+      </c>
+      <c r="M47" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>165</v>
+      </c>
+      <c r="F48" t="s">
+        <v>238</v>
+      </c>
+      <c r="G48" t="s">
+        <v>239</v>
+      </c>
+      <c r="H48" t="s">
+        <v>239</v>
+      </c>
+      <c r="I48" t="s">
+        <v>239</v>
+      </c>
+      <c r="J48" t="s">
+        <v>239</v>
+      </c>
+      <c r="K48" t="s">
+        <v>239</v>
+      </c>
+      <c r="L48" t="s">
+        <v>239</v>
+      </c>
+      <c r="M48" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>172</v>
+      </c>
+      <c r="G49" t="s">
+        <v>238</v>
+      </c>
+      <c r="H49" t="s">
+        <v>239</v>
+      </c>
+      <c r="I49" t="s">
+        <v>239</v>
+      </c>
+      <c r="J49" t="s">
+        <v>239</v>
+      </c>
+      <c r="K49" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="G50" t="s">
+        <v>238</v>
+      </c>
+      <c r="H50" t="s">
+        <v>239</v>
+      </c>
+      <c r="I50" t="s">
+        <v>239</v>
+      </c>
+      <c r="J50" t="s">
+        <v>239</v>
+      </c>
+      <c r="K50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="I51" t="s">
+        <v>238</v>
+      </c>
+      <c r="J51" t="s">
+        <v>239</v>
+      </c>
+      <c r="K51" t="s">
+        <v>239</v>
+      </c>
+      <c r="L51" t="s">
+        <v>239</v>
+      </c>
+      <c r="M51" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" t="s">
+        <v>238</v>
+      </c>
+      <c r="F52" t="s">
+        <v>239</v>
+      </c>
+      <c r="G52" t="s">
+        <v>237</v>
+      </c>
+      <c r="K52" t="s">
+        <v>238</v>
+      </c>
+      <c r="L52" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>162</v>
+      </c>
+      <c r="H53" t="s">
+        <v>238</v>
+      </c>
+      <c r="I53" t="s">
+        <v>239</v>
+      </c>
+      <c r="J53" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>330</v>
+      </c>
+      <c r="E54" t="s">
+        <v>238</v>
+      </c>
+      <c r="F54" t="s">
+        <v>239</v>
+      </c>
+      <c r="G54" t="s">
+        <v>237</v>
+      </c>
+      <c r="J54" t="s">
+        <v>238</v>
+      </c>
+      <c r="K54" t="s">
+        <v>239</v>
+      </c>
+      <c r="L54" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>298</v>
+      </c>
+      <c r="H55" t="s">
+        <v>238</v>
+      </c>
+      <c r="I55" t="s">
+        <v>239</v>
+      </c>
+      <c r="J55" t="s">
+        <v>239</v>
+      </c>
+      <c r="K55" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>334</v>
+      </c>
+      <c r="H56" t="s">
+        <v>238</v>
+      </c>
+      <c r="I56" t="s">
+        <v>239</v>
+      </c>
+      <c r="J56" t="s">
+        <v>239</v>
+      </c>
+      <c r="K56" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" t="s">
+        <v>238</v>
+      </c>
+      <c r="F57" t="s">
+        <v>239</v>
+      </c>
+      <c r="G57" t="s">
+        <v>237</v>
+      </c>
+      <c r="J57" t="s">
+        <v>238</v>
+      </c>
+      <c r="K57" t="s">
+        <v>239</v>
+      </c>
+      <c r="L57" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC17C640-AEF4-498F-990E-5958CA65631E}">
+  <dimension ref="B1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9A47CA-EEF1-4151-A46A-9938347DBA49}">
+  <dimension ref="A1:M53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="17.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E2" t="s">
+        <v>338</v>
+      </c>
+      <c r="F2" t="s">
+        <v>338</v>
+      </c>
+      <c r="G2" t="s">
+        <v>338</v>
+      </c>
+      <c r="H2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L2" t="s">
+        <v>237</v>
+      </c>
+      <c r="M2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>238</v>
+      </c>
+      <c r="J3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I4" t="s">
+        <v>239</v>
+      </c>
+      <c r="J4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>238</v>
+      </c>
+      <c r="J5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>326</v>
+      </c>
+      <c r="I7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" t="s">
+        <v>238</v>
+      </c>
+      <c r="J8" t="s">
+        <v>239</v>
+      </c>
+      <c r="K8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>238</v>
+      </c>
+      <c r="I9" t="s">
+        <v>239</v>
+      </c>
+      <c r="J9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>338</v>
+      </c>
+      <c r="C10" t="s">
+        <v>338</v>
+      </c>
+      <c r="I10" t="s">
+        <v>238</v>
+      </c>
+      <c r="J10" t="s">
+        <v>239</v>
+      </c>
+      <c r="K10" t="s">
+        <v>237</v>
+      </c>
+      <c r="L10" t="s">
+        <v>338</v>
+      </c>
+      <c r="M10" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" t="s">
+        <v>238</v>
+      </c>
+      <c r="I11" t="s">
+        <v>239</v>
+      </c>
+      <c r="J11" t="s">
+        <v>237</v>
+      </c>
+      <c r="K11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>150</v>
+      </c>
+      <c r="I12" t="s">
+        <v>238</v>
+      </c>
+      <c r="J12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
+        <v>239</v>
+      </c>
+      <c r="J13" t="s">
+        <v>238</v>
+      </c>
+      <c r="K13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" t="s">
+        <v>238</v>
+      </c>
+      <c r="K15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" t="s">
+        <v>238</v>
+      </c>
+      <c r="G16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+      <c r="B17" t="s">
+        <v>338</v>
+      </c>
+      <c r="C17" t="s">
+        <v>338</v>
+      </c>
+      <c r="D17" t="s">
+        <v>338</v>
+      </c>
+      <c r="E17" t="s">
+        <v>338</v>
+      </c>
+      <c r="F17" t="s">
+        <v>338</v>
+      </c>
+      <c r="G17" t="s">
+        <v>338</v>
+      </c>
+      <c r="H17" t="s">
+        <v>338</v>
+      </c>
+      <c r="I17" t="s">
+        <v>338</v>
+      </c>
+      <c r="J17" t="s">
+        <v>238</v>
+      </c>
+      <c r="K17" t="s">
+        <v>239</v>
+      </c>
+      <c r="L17" t="s">
+        <v>239</v>
+      </c>
+      <c r="M17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>336</v>
+      </c>
+      <c r="J18" t="s">
+        <v>238</v>
+      </c>
+      <c r="K18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>337</v>
+      </c>
+      <c r="H19" t="s">
+        <v>238</v>
+      </c>
+      <c r="I19" t="s">
+        <v>239</v>
+      </c>
+      <c r="J19" t="s">
+        <v>239</v>
+      </c>
+      <c r="K19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>338</v>
+      </c>
+      <c r="C20" t="s">
+        <v>338</v>
+      </c>
+      <c r="G20" t="s">
+        <v>238</v>
+      </c>
+      <c r="H20" t="s">
+        <v>239</v>
+      </c>
+      <c r="I20" t="s">
+        <v>239</v>
+      </c>
+      <c r="J20" t="s">
+        <v>239</v>
+      </c>
+      <c r="K20" t="s">
+        <v>239</v>
+      </c>
+      <c r="L20" t="s">
+        <v>237</v>
+      </c>
+      <c r="M20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>286</v>
+      </c>
+      <c r="F21" t="s">
+        <v>238</v>
+      </c>
+      <c r="G21" t="s">
+        <v>239</v>
+      </c>
+      <c r="H21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I21" t="s">
+        <v>239</v>
+      </c>
+      <c r="J21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>238</v>
+      </c>
+      <c r="H22" t="s">
+        <v>239</v>
+      </c>
+      <c r="I22" t="s">
+        <v>239</v>
+      </c>
+      <c r="J22" t="s">
+        <v>239</v>
+      </c>
+      <c r="K22" t="s">
+        <v>239</v>
+      </c>
+      <c r="L22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J23" t="s">
+        <v>238</v>
+      </c>
+      <c r="K23" t="s">
+        <v>239</v>
+      </c>
+      <c r="L23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>338</v>
+      </c>
+      <c r="C24" t="s">
+        <v>338</v>
+      </c>
+      <c r="D24" t="s">
+        <v>338</v>
+      </c>
+      <c r="G24" t="s">
+        <v>238</v>
+      </c>
+      <c r="H24" t="s">
+        <v>239</v>
+      </c>
+      <c r="I24" t="s">
+        <v>239</v>
+      </c>
+      <c r="J24" t="s">
+        <v>239</v>
+      </c>
+      <c r="K24" t="s">
+        <v>239</v>
+      </c>
+      <c r="L24" t="s">
+        <v>239</v>
+      </c>
+      <c r="M24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>338</v>
+      </c>
+      <c r="C25" t="s">
+        <v>338</v>
+      </c>
+      <c r="D25" t="s">
+        <v>338</v>
+      </c>
+      <c r="E25" t="s">
+        <v>338</v>
+      </c>
+      <c r="H25" t="s">
+        <v>238</v>
+      </c>
+      <c r="I25" t="s">
+        <v>239</v>
+      </c>
+      <c r="J25" t="s">
+        <v>239</v>
+      </c>
+      <c r="K25" t="s">
+        <v>239</v>
+      </c>
+      <c r="L25" t="s">
+        <v>237</v>
+      </c>
+      <c r="M25" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" t="s">
+        <v>238</v>
+      </c>
+      <c r="J26" t="s">
+        <v>239</v>
+      </c>
+      <c r="K26" t="s">
+        <v>239</v>
+      </c>
+      <c r="L26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" t="s">
+        <v>238</v>
+      </c>
+      <c r="J27" t="s">
+        <v>239</v>
+      </c>
+      <c r="K27" t="s">
+        <v>239</v>
+      </c>
+      <c r="L27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" t="s">
+        <v>238</v>
+      </c>
+      <c r="I28" t="s">
+        <v>239</v>
+      </c>
+      <c r="J28" t="s">
+        <v>239</v>
+      </c>
+      <c r="K28" t="s">
+        <v>239</v>
+      </c>
+      <c r="L28" t="s">
+        <v>239</v>
+      </c>
+      <c r="M28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" t="s">
+        <v>238</v>
+      </c>
+      <c r="J29" t="s">
+        <v>239</v>
+      </c>
+      <c r="K29" t="s">
+        <v>239</v>
+      </c>
+      <c r="L29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" t="s">
+        <v>238</v>
+      </c>
+      <c r="I30" t="s">
+        <v>239</v>
+      </c>
+      <c r="J30" t="s">
+        <v>239</v>
+      </c>
+      <c r="K30" t="s">
+        <v>239</v>
+      </c>
+      <c r="L30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" t="s">
+        <v>238</v>
+      </c>
+      <c r="J31" t="s">
+        <v>239</v>
+      </c>
+      <c r="K31" t="s">
+        <v>239</v>
+      </c>
+      <c r="L31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>137</v>
+      </c>
+      <c r="G32" t="s">
+        <v>238</v>
+      </c>
+      <c r="H32" t="s">
+        <v>237</v>
+      </c>
+      <c r="I32" t="s">
+        <v>338</v>
+      </c>
+      <c r="J32" t="s">
+        <v>338</v>
+      </c>
+      <c r="K32" t="s">
+        <v>338</v>
+      </c>
+      <c r="L32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>338</v>
+      </c>
+      <c r="C33" t="s">
+        <v>338</v>
+      </c>
+      <c r="D33" t="s">
+        <v>338</v>
+      </c>
+      <c r="E33" t="s">
+        <v>338</v>
+      </c>
+      <c r="F33" t="s">
+        <v>338</v>
+      </c>
+      <c r="G33" t="s">
+        <v>238</v>
+      </c>
+      <c r="H33" t="s">
+        <v>239</v>
+      </c>
+      <c r="I33" t="s">
+        <v>239</v>
+      </c>
+      <c r="J33" t="s">
+        <v>239</v>
+      </c>
+      <c r="K33" t="s">
+        <v>237</v>
+      </c>
+      <c r="L33" t="s">
+        <v>338</v>
+      </c>
+      <c r="M33" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" t="s">
+        <v>238</v>
+      </c>
+      <c r="J34" t="s">
+        <v>239</v>
+      </c>
+      <c r="K34" t="s">
+        <v>239</v>
+      </c>
+      <c r="L34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35" t="s">
+        <v>238</v>
+      </c>
+      <c r="J35" t="s">
+        <v>239</v>
+      </c>
+      <c r="K35" t="s">
+        <v>237</v>
+      </c>
+      <c r="L35" t="s">
+        <v>338</v>
+      </c>
+      <c r="M35" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>238</v>
+      </c>
+      <c r="G36" t="s">
+        <v>239</v>
+      </c>
+      <c r="H36" t="s">
+        <v>239</v>
+      </c>
+      <c r="I36" t="s">
+        <v>239</v>
+      </c>
+      <c r="J36" t="s">
+        <v>239</v>
+      </c>
+      <c r="K36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>316</v>
+      </c>
+      <c r="G37" t="s">
+        <v>238</v>
+      </c>
+      <c r="H37" t="s">
+        <v>239</v>
+      </c>
+      <c r="I37" t="s">
+        <v>239</v>
+      </c>
+      <c r="J37" t="s">
+        <v>239</v>
+      </c>
+      <c r="K37" t="s">
+        <v>239</v>
+      </c>
+      <c r="L37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>338</v>
+      </c>
+      <c r="C38" t="s">
+        <v>338</v>
+      </c>
+      <c r="D38" t="s">
+        <v>338</v>
+      </c>
+      <c r="E38" t="s">
+        <v>338</v>
+      </c>
+      <c r="F38" t="s">
+        <v>338</v>
+      </c>
+      <c r="G38" t="s">
+        <v>338</v>
+      </c>
+      <c r="H38" t="s">
+        <v>238</v>
+      </c>
+      <c r="I38" t="s">
+        <v>239</v>
+      </c>
+      <c r="J38" t="s">
+        <v>239</v>
+      </c>
+      <c r="K38" t="s">
+        <v>239</v>
+      </c>
+      <c r="L38" t="s">
+        <v>237</v>
+      </c>
+      <c r="M38" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="s">
+        <v>338</v>
+      </c>
+      <c r="C39" t="s">
+        <v>338</v>
+      </c>
+      <c r="D39" t="s">
+        <v>338</v>
+      </c>
+      <c r="E39" t="s">
+        <v>238</v>
+      </c>
+      <c r="F39" t="s">
+        <v>237</v>
+      </c>
+      <c r="K39" t="s">
+        <v>238</v>
+      </c>
+      <c r="L39" t="s">
+        <v>239</v>
+      </c>
+      <c r="M39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="G40" t="s">
+        <v>238</v>
+      </c>
+      <c r="H40" t="s">
+        <v>237</v>
+      </c>
+      <c r="J40" t="s">
+        <v>238</v>
+      </c>
+      <c r="K40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" t="s">
+        <v>238</v>
+      </c>
+      <c r="I41" t="s">
+        <v>239</v>
+      </c>
+      <c r="J41" t="s">
+        <v>239</v>
+      </c>
+      <c r="K41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>338</v>
+      </c>
+      <c r="C42" t="s">
+        <v>338</v>
+      </c>
+      <c r="D42" t="s">
+        <v>338</v>
+      </c>
+      <c r="E42" t="s">
+        <v>338</v>
+      </c>
+      <c r="F42" t="s">
+        <v>338</v>
+      </c>
+      <c r="G42" t="s">
+        <v>338</v>
+      </c>
+      <c r="H42" t="s">
+        <v>238</v>
+      </c>
+      <c r="I42" t="s">
+        <v>239</v>
+      </c>
+      <c r="J42" t="s">
+        <v>239</v>
+      </c>
+      <c r="K42" t="s">
+        <v>237</v>
+      </c>
+      <c r="L42" t="s">
+        <v>338</v>
+      </c>
+      <c r="M42" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+      <c r="J43" t="s">
+        <v>238</v>
+      </c>
+      <c r="K43" t="s">
+        <v>237</v>
+      </c>
+      <c r="L43" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" t="s">
+        <v>238</v>
+      </c>
+      <c r="G44" t="s">
+        <v>239</v>
+      </c>
+      <c r="H44" t="s">
+        <v>239</v>
+      </c>
+      <c r="I44" t="s">
+        <v>239</v>
+      </c>
+      <c r="J44" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" t="s">
+        <v>238</v>
+      </c>
+      <c r="G45" t="s">
+        <v>239</v>
+      </c>
+      <c r="H45" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" t="s">
+        <v>238</v>
+      </c>
+      <c r="G46" t="s">
+        <v>239</v>
+      </c>
+      <c r="H46" t="s">
+        <v>239</v>
+      </c>
+      <c r="I46" t="s">
+        <v>239</v>
+      </c>
+      <c r="J46" t="s">
+        <v>239</v>
+      </c>
+      <c r="K46" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>161</v>
+      </c>
+      <c r="G47" t="s">
+        <v>238</v>
+      </c>
+      <c r="H47" t="s">
+        <v>239</v>
+      </c>
+      <c r="I47" t="s">
+        <v>239</v>
+      </c>
+      <c r="J47" t="s">
+        <v>239</v>
+      </c>
+      <c r="K47" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>338</v>
+      </c>
+      <c r="C48" t="s">
+        <v>338</v>
+      </c>
+      <c r="I48" t="s">
+        <v>238</v>
+      </c>
+      <c r="J48" t="s">
+        <v>239</v>
+      </c>
+      <c r="K48" t="s">
+        <v>239</v>
+      </c>
+      <c r="L48" t="s">
+        <v>237</v>
+      </c>
+      <c r="M48" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>104</v>
+      </c>
+      <c r="G49" t="s">
+        <v>238</v>
+      </c>
+      <c r="H49" t="s">
+        <v>239</v>
+      </c>
+      <c r="I49" t="s">
+        <v>239</v>
+      </c>
+      <c r="J49" t="s">
+        <v>239</v>
+      </c>
+      <c r="K49" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" t="s">
+        <v>238</v>
+      </c>
+      <c r="H50" t="s">
+        <v>239</v>
+      </c>
+      <c r="I50" t="s">
+        <v>239</v>
+      </c>
+      <c r="J50" t="s">
+        <v>239</v>
+      </c>
+      <c r="K50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>338</v>
+      </c>
+      <c r="C51" t="s">
+        <v>338</v>
+      </c>
+      <c r="D51" t="s">
+        <v>338</v>
+      </c>
+      <c r="I51" t="s">
+        <v>238</v>
+      </c>
+      <c r="J51" t="s">
+        <v>239</v>
+      </c>
+      <c r="K51" t="s">
+        <v>239</v>
+      </c>
+      <c r="L51" t="s">
+        <v>237</v>
+      </c>
+      <c r="M51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>311</v>
+      </c>
+      <c r="F52" t="s">
+        <v>238</v>
+      </c>
+      <c r="G52" t="s">
+        <v>239</v>
+      </c>
+      <c r="H52" t="s">
+        <v>239</v>
+      </c>
+      <c r="I52" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="G53" t="s">
+        <v>238</v>
+      </c>
+      <c r="H53" t="s">
+        <v>239</v>
+      </c>
+      <c r="I53" t="s">
+        <v>239</v>
+      </c>
+      <c r="J53" t="s">
+        <v>239</v>
+      </c>
+      <c r="K53" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5F2BCB-E954-4FB3-9902-5D527AA48DE9}">
+  <dimension ref="A1:M59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L2" t="s">
+        <v>239</v>
+      </c>
+      <c r="M2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" t="s">
+        <v>237</v>
+      </c>
+      <c r="K4" t="s">
+        <v>238</v>
+      </c>
+      <c r="L4" t="s">
+        <v>239</v>
+      </c>
+      <c r="M4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>238</v>
+      </c>
+      <c r="G6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>339</v>
+      </c>
+      <c r="F7" t="s">
+        <v>238</v>
+      </c>
+      <c r="G7" t="s">
+        <v>237</v>
+      </c>
+      <c r="K7" t="s">
+        <v>238</v>
+      </c>
+      <c r="L7" t="s">
+        <v>239</v>
+      </c>
+      <c r="M7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>238</v>
+      </c>
+      <c r="F8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>340</v>
+      </c>
+      <c r="H9" t="s">
+        <v>238</v>
+      </c>
+      <c r="I9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>238</v>
+      </c>
+      <c r="G10" t="s">
+        <v>239</v>
+      </c>
+      <c r="H10" t="s">
+        <v>239</v>
+      </c>
+      <c r="I10" t="s">
+        <v>239</v>
+      </c>
+      <c r="J10" t="s">
+        <v>239</v>
+      </c>
+      <c r="K10" t="s">
+        <v>239</v>
+      </c>
+      <c r="L10" t="s">
+        <v>239</v>
+      </c>
+      <c r="M10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>238</v>
+      </c>
+      <c r="I11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>237</v>
+      </c>
+      <c r="G12" t="s">
+        <v>238</v>
+      </c>
+      <c r="H12" t="s">
+        <v>237</v>
+      </c>
+      <c r="M12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>298</v>
+      </c>
+      <c r="H13" t="s">
+        <v>238</v>
+      </c>
+      <c r="I13" t="s">
+        <v>239</v>
+      </c>
+      <c r="J13" t="s">
+        <v>239</v>
+      </c>
+      <c r="K13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D14" t="s">
+        <v>239</v>
+      </c>
+      <c r="E14" t="s">
+        <v>239</v>
+      </c>
+      <c r="F14" t="s">
+        <v>239</v>
+      </c>
+      <c r="G14" t="s">
+        <v>239</v>
+      </c>
+      <c r="H14" t="s">
+        <v>239</v>
+      </c>
+      <c r="I14" t="s">
+        <v>239</v>
+      </c>
+      <c r="J14" t="s">
+        <v>239</v>
+      </c>
+      <c r="K14" t="s">
+        <v>239</v>
+      </c>
+      <c r="L14" t="s">
+        <v>239</v>
+      </c>
+      <c r="M14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>238</v>
+      </c>
+      <c r="H15" t="s">
+        <v>239</v>
+      </c>
+      <c r="I15" t="s">
+        <v>239</v>
+      </c>
+      <c r="J15" t="s">
+        <v>239</v>
+      </c>
+      <c r="K15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>238</v>
+      </c>
+      <c r="H16" t="s">
+        <v>239</v>
+      </c>
+      <c r="I16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" t="s">
+        <v>238</v>
+      </c>
+      <c r="I17" t="s">
+        <v>239</v>
+      </c>
+      <c r="J17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H18" t="s">
+        <v>238</v>
+      </c>
+      <c r="I18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="G19" t="s">
+        <v>238</v>
+      </c>
+      <c r="H19" t="s">
+        <v>239</v>
+      </c>
+      <c r="I19" t="s">
+        <v>239</v>
+      </c>
+      <c r="J19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+      <c r="F20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+      <c r="D21" t="s">
+        <v>238</v>
+      </c>
+      <c r="E21" t="s">
+        <v>239</v>
+      </c>
+      <c r="F21" t="s">
+        <v>239</v>
+      </c>
+      <c r="G21" t="s">
+        <v>239</v>
+      </c>
+      <c r="H21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I21" t="s">
+        <v>239</v>
+      </c>
+      <c r="J21" t="s">
+        <v>239</v>
+      </c>
+      <c r="K21" t="s">
+        <v>239</v>
+      </c>
+      <c r="L21" t="s">
+        <v>239</v>
+      </c>
+      <c r="M21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>239</v>
+      </c>
+      <c r="C22" t="s">
+        <v>239</v>
+      </c>
+      <c r="D22" t="s">
+        <v>239</v>
+      </c>
+      <c r="E22" t="s">
+        <v>239</v>
+      </c>
+      <c r="F22" t="s">
+        <v>239</v>
+      </c>
+      <c r="G22" t="s">
+        <v>239</v>
+      </c>
+      <c r="H22" t="s">
+        <v>239</v>
+      </c>
+      <c r="I22" t="s">
+        <v>239</v>
+      </c>
+      <c r="J22" t="s">
+        <v>239</v>
+      </c>
+      <c r="K22" t="s">
+        <v>239</v>
+      </c>
+      <c r="L22" t="s">
+        <v>239</v>
+      </c>
+      <c r="M22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+      <c r="H23" t="s">
+        <v>238</v>
+      </c>
+      <c r="I23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+      <c r="J24" t="s">
+        <v>238</v>
+      </c>
+      <c r="K24" t="s">
+        <v>239</v>
+      </c>
+      <c r="L24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>238</v>
+      </c>
+      <c r="G25" t="s">
+        <v>237</v>
+      </c>
+      <c r="K25" t="s">
+        <v>238</v>
+      </c>
+      <c r="L25" t="s">
+        <v>239</v>
+      </c>
+      <c r="M25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>238</v>
+      </c>
+      <c r="F26" t="s">
+        <v>237</v>
+      </c>
+      <c r="K26" t="s">
+        <v>238</v>
+      </c>
+      <c r="L26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+        <v>343</v>
+      </c>
+      <c r="I27" t="s">
+        <v>238</v>
+      </c>
+      <c r="J27" t="s">
+        <v>239</v>
+      </c>
+      <c r="K27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+      <c r="D28" t="s">
+        <v>238</v>
+      </c>
+      <c r="E28" t="s">
+        <v>239</v>
+      </c>
+      <c r="F28" t="s">
+        <v>239</v>
+      </c>
+      <c r="G28" t="s">
+        <v>237</v>
+      </c>
+      <c r="J28" t="s">
+        <v>238</v>
+      </c>
+      <c r="K28" t="s">
+        <v>239</v>
+      </c>
+      <c r="L28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+      <c r="E29" t="s">
+        <v>238</v>
+      </c>
+      <c r="F29" t="s">
+        <v>239</v>
+      </c>
+      <c r="G29" t="s">
+        <v>237</v>
+      </c>
+      <c r="J29" t="s">
+        <v>238</v>
+      </c>
+      <c r="K29" t="s">
+        <v>239</v>
+      </c>
+      <c r="L29" t="s">
+        <v>239</v>
+      </c>
+      <c r="M29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="F30" t="s">
+        <v>238</v>
+      </c>
+      <c r="G30" t="s">
+        <v>237</v>
+      </c>
+      <c r="K30" t="s">
+        <v>238</v>
+      </c>
+      <c r="L30" t="s">
+        <v>239</v>
+      </c>
+      <c r="M30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+      <c r="H31" t="s">
+        <v>238</v>
+      </c>
+      <c r="I31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="H32" t="s">
+        <v>238</v>
+      </c>
+      <c r="I32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G33" t="s">
+        <v>238</v>
+      </c>
+      <c r="H33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="G34" t="s">
+        <v>238</v>
+      </c>
+      <c r="H34" t="s">
+        <v>239</v>
+      </c>
+      <c r="I34" t="s">
+        <v>239</v>
+      </c>
+      <c r="J34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+      <c r="B35" t="s">
+        <v>239</v>
+      </c>
+      <c r="C35" t="s">
+        <v>239</v>
+      </c>
+      <c r="D35" t="s">
+        <v>239</v>
+      </c>
+      <c r="E35" t="s">
+        <v>239</v>
+      </c>
+      <c r="F35" t="s">
+        <v>239</v>
+      </c>
+      <c r="G35" t="s">
+        <v>239</v>
+      </c>
+      <c r="H35" t="s">
+        <v>239</v>
+      </c>
+      <c r="I35" t="s">
+        <v>239</v>
+      </c>
+      <c r="J35" t="s">
+        <v>239</v>
+      </c>
+      <c r="K35" t="s">
+        <v>239</v>
+      </c>
+      <c r="L35" t="s">
+        <v>239</v>
+      </c>
+      <c r="M35" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="I36" t="s">
+        <v>238</v>
+      </c>
+      <c r="J36" t="s">
+        <v>239</v>
+      </c>
+      <c r="K36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="L37" t="s">
+        <v>238</v>
+      </c>
+      <c r="M37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="G38" t="s">
+        <v>238</v>
+      </c>
+      <c r="H38" t="s">
+        <v>239</v>
+      </c>
+      <c r="I38" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="J39" t="s">
+        <v>238</v>
+      </c>
+      <c r="K39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="G40" t="s">
+        <v>238</v>
+      </c>
+      <c r="H40" t="s">
+        <v>239</v>
+      </c>
+      <c r="I40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>238</v>
+      </c>
+      <c r="H41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="J42" t="s">
+        <v>238</v>
+      </c>
+      <c r="K42" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="E43" t="s">
+        <v>238</v>
+      </c>
+      <c r="F43" t="s">
+        <v>239</v>
+      </c>
+      <c r="G43" t="s">
+        <v>237</v>
+      </c>
+      <c r="K43" t="s">
+        <v>238</v>
+      </c>
+      <c r="L43" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="G44" t="s">
+        <v>239</v>
+      </c>
+      <c r="J44" t="s">
+        <v>238</v>
+      </c>
+      <c r="K44" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+      <c r="E45" t="s">
+        <v>238</v>
+      </c>
+      <c r="F45" t="s">
+        <v>237</v>
+      </c>
+      <c r="K45" t="s">
+        <v>238</v>
+      </c>
+      <c r="L45" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>111</v>
+      </c>
+      <c r="G46" t="s">
+        <v>238</v>
+      </c>
+      <c r="H46" t="s">
+        <v>239</v>
+      </c>
+      <c r="I46" t="s">
+        <v>239</v>
+      </c>
+      <c r="J46" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>345</v>
+      </c>
+      <c r="F47" t="s">
+        <v>238</v>
+      </c>
+      <c r="G47" t="s">
+        <v>239</v>
+      </c>
+      <c r="K47" t="s">
+        <v>238</v>
+      </c>
+      <c r="L47" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>346</v>
+      </c>
+      <c r="E48" t="s">
+        <v>238</v>
+      </c>
+      <c r="F48" t="s">
+        <v>237</v>
+      </c>
+      <c r="K48" t="s">
+        <v>238</v>
+      </c>
+      <c r="L48" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>239</v>
+      </c>
+      <c r="C49" t="s">
+        <v>239</v>
+      </c>
+      <c r="D49" t="s">
+        <v>239</v>
+      </c>
+      <c r="E49" t="s">
+        <v>239</v>
+      </c>
+      <c r="F49" t="s">
+        <v>237</v>
+      </c>
+      <c r="K49" t="s">
+        <v>238</v>
+      </c>
+      <c r="L49" t="s">
+        <v>239</v>
+      </c>
+      <c r="M49" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>347</v>
+      </c>
+      <c r="H50" t="s">
+        <v>238</v>
+      </c>
+      <c r="I50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>172</v>
+      </c>
+      <c r="F51" t="s">
+        <v>238</v>
+      </c>
+      <c r="G51" t="s">
+        <v>239</v>
+      </c>
+      <c r="H51" t="s">
+        <v>239</v>
+      </c>
+      <c r="I51" t="s">
+        <v>239</v>
+      </c>
+      <c r="J51" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>238</v>
+      </c>
+      <c r="F52" t="s">
+        <v>239</v>
+      </c>
+      <c r="G52" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>162</v>
+      </c>
+      <c r="G53" t="s">
+        <v>238</v>
+      </c>
+      <c r="H53" t="s">
+        <v>239</v>
+      </c>
+      <c r="I53" t="s">
+        <v>239</v>
+      </c>
+      <c r="J53" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>167</v>
+      </c>
+      <c r="B54" t="s">
+        <v>239</v>
+      </c>
+      <c r="C54" t="s">
+        <v>239</v>
+      </c>
+      <c r="D54" t="s">
+        <v>239</v>
+      </c>
+      <c r="E54" t="s">
+        <v>239</v>
+      </c>
+      <c r="F54" t="s">
+        <v>239</v>
+      </c>
+      <c r="G54" t="s">
+        <v>239</v>
+      </c>
+      <c r="H54" t="s">
+        <v>239</v>
+      </c>
+      <c r="I54" t="s">
+        <v>239</v>
+      </c>
+      <c r="J54" t="s">
+        <v>239</v>
+      </c>
+      <c r="K54" t="s">
+        <v>239</v>
+      </c>
+      <c r="L54" t="s">
+        <v>239</v>
+      </c>
+      <c r="M54" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" t="s">
+        <v>238</v>
+      </c>
+      <c r="H55" t="s">
+        <v>239</v>
+      </c>
+      <c r="I55" t="s">
+        <v>239</v>
+      </c>
+      <c r="J55" t="s">
+        <v>239</v>
+      </c>
+      <c r="K55" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>154</v>
+      </c>
+      <c r="G56" t="s">
+        <v>238</v>
+      </c>
+      <c r="H56" t="s">
+        <v>239</v>
+      </c>
+      <c r="I56" t="s">
+        <v>239</v>
+      </c>
+      <c r="J56" t="s">
+        <v>239</v>
+      </c>
+      <c r="K56" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" t="s">
+        <v>238</v>
+      </c>
+      <c r="F57" t="s">
+        <v>239</v>
+      </c>
+      <c r="G57" t="s">
+        <v>237</v>
+      </c>
+      <c r="K57" t="s">
+        <v>238</v>
+      </c>
+      <c r="L57" t="s">
+        <v>239</v>
+      </c>
+      <c r="M57" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>127</v>
+      </c>
+      <c r="H58" t="s">
+        <v>238</v>
+      </c>
+      <c r="I58" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>51</v>
+      </c>
+      <c r="F59" t="s">
+        <v>238</v>
+      </c>
+      <c r="G59" t="s">
+        <v>239</v>
+      </c>
+      <c r="H59" t="s">
+        <v>239</v>
+      </c>
+      <c r="I59" t="s">
+        <v>239</v>
+      </c>
+      <c r="J59" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A1634EA-A489-4A13-B66B-6FBA758233DF}">
+  <dimension ref="A1:M49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>238</v>
+      </c>
+      <c r="I3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>348</v>
+      </c>
+      <c r="I4" t="s">
+        <v>238</v>
+      </c>
+      <c r="J4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>326</v>
+      </c>
+      <c r="G5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>349</v>
+      </c>
+      <c r="H7" t="s">
+        <v>238</v>
+      </c>
+      <c r="I7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" t="s">
+        <v>238</v>
+      </c>
+      <c r="J8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>238</v>
+      </c>
+      <c r="I9" t="s">
+        <v>239</v>
+      </c>
+      <c r="J9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>238</v>
+      </c>
+      <c r="G10" t="s">
+        <v>239</v>
+      </c>
+      <c r="H10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>238</v>
+      </c>
+      <c r="H11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" t="s">
+        <v>238</v>
+      </c>
+      <c r="G12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
+        <v>238</v>
+      </c>
+      <c r="I13" t="s">
+        <v>239</v>
+      </c>
+      <c r="J13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H14" t="s">
+        <v>239</v>
+      </c>
+      <c r="I14" t="s">
+        <v>239</v>
+      </c>
+      <c r="J14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>238</v>
+      </c>
+      <c r="H15" t="s">
+        <v>239</v>
+      </c>
+      <c r="I15" t="s">
+        <v>239</v>
+      </c>
+      <c r="J15" t="s">
+        <v>239</v>
+      </c>
+      <c r="K15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" t="s">
+        <v>238</v>
+      </c>
+      <c r="K16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" t="s">
+        <v>238</v>
+      </c>
+      <c r="I17" t="s">
+        <v>239</v>
+      </c>
+      <c r="J17" t="s">
+        <v>239</v>
+      </c>
+      <c r="K17" t="s">
+        <v>239</v>
+      </c>
+      <c r="L17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" t="s">
+        <v>238</v>
+      </c>
+      <c r="I18" t="s">
+        <v>239</v>
+      </c>
+      <c r="J18" t="s">
+        <v>239</v>
+      </c>
+      <c r="K18" t="s">
+        <v>239</v>
+      </c>
+      <c r="L18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" t="s">
+        <v>238</v>
+      </c>
+      <c r="J19" t="s">
+        <v>239</v>
+      </c>
+      <c r="K19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>238</v>
+      </c>
+      <c r="I21" t="s">
+        <v>239</v>
+      </c>
+      <c r="J21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" t="s">
+        <v>238</v>
+      </c>
+      <c r="I22" t="s">
+        <v>239</v>
+      </c>
+      <c r="J22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" t="s">
+        <v>238</v>
+      </c>
+      <c r="J23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>270</v>
+      </c>
+      <c r="G24" t="s">
+        <v>238</v>
+      </c>
+      <c r="H24" t="s">
+        <v>239</v>
+      </c>
+      <c r="I24" t="s">
+        <v>239</v>
+      </c>
+      <c r="J24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>216</v>
+      </c>
+      <c r="G25" t="s">
+        <v>238</v>
+      </c>
+      <c r="H25" t="s">
+        <v>239</v>
+      </c>
+      <c r="I25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>238</v>
+      </c>
+      <c r="F26" t="s">
+        <v>239</v>
+      </c>
+      <c r="G26" t="s">
+        <v>239</v>
+      </c>
+      <c r="H26" t="s">
+        <v>239</v>
+      </c>
+      <c r="I26" t="s">
+        <v>239</v>
+      </c>
+      <c r="J26" t="s">
+        <v>239</v>
+      </c>
+      <c r="K26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" t="s">
+        <v>238</v>
+      </c>
+      <c r="H27" t="s">
+        <v>239</v>
+      </c>
+      <c r="I27" t="s">
+        <v>239</v>
+      </c>
+      <c r="J27" t="s">
+        <v>239</v>
+      </c>
+      <c r="K27" t="s">
+        <v>239</v>
+      </c>
+      <c r="L27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" t="s">
+        <v>238</v>
+      </c>
+      <c r="H28" t="s">
+        <v>239</v>
+      </c>
+      <c r="I28" t="s">
+        <v>239</v>
+      </c>
+      <c r="J28" t="s">
+        <v>239</v>
+      </c>
+      <c r="K28" t="s">
+        <v>239</v>
+      </c>
+      <c r="L28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>238</v>
+      </c>
+      <c r="F29" t="s">
+        <v>239</v>
+      </c>
+      <c r="G29" t="s">
+        <v>239</v>
+      </c>
+      <c r="H29" t="s">
+        <v>239</v>
+      </c>
+      <c r="I29" t="s">
+        <v>239</v>
+      </c>
+      <c r="J29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>350</v>
+      </c>
+      <c r="I30" t="s">
+        <v>238</v>
+      </c>
+      <c r="J30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>157</v>
+      </c>
+      <c r="G31" t="s">
+        <v>238</v>
+      </c>
+      <c r="H31" t="s">
+        <v>239</v>
+      </c>
+      <c r="I31" t="s">
+        <v>239</v>
+      </c>
+      <c r="J31" t="s">
+        <v>239</v>
+      </c>
+      <c r="K31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="I32" t="s">
+        <v>238</v>
+      </c>
+      <c r="J32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" t="s">
+        <v>238</v>
+      </c>
+      <c r="J33" t="s">
+        <v>239</v>
+      </c>
+      <c r="K33" t="s">
+        <v>239</v>
+      </c>
+      <c r="L33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" t="s">
+        <v>238</v>
+      </c>
+      <c r="H34" t="s">
+        <v>239</v>
+      </c>
+      <c r="I34" t="s">
+        <v>239</v>
+      </c>
+      <c r="J34" t="s">
+        <v>239</v>
+      </c>
+      <c r="K34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="J35" t="s">
+        <v>238</v>
+      </c>
+      <c r="K35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" t="s">
+        <v>238</v>
+      </c>
+      <c r="G36" t="s">
+        <v>239</v>
+      </c>
+      <c r="H36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" t="s">
+        <v>238</v>
+      </c>
+      <c r="I37" t="s">
+        <v>239</v>
+      </c>
+      <c r="J37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" t="s">
+        <v>238</v>
+      </c>
+      <c r="J38" t="s">
+        <v>239</v>
+      </c>
+      <c r="K38" t="s">
+        <v>239</v>
+      </c>
+      <c r="L38" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="J39" t="s">
+        <v>238</v>
+      </c>
+      <c r="K39" t="s">
+        <v>239</v>
+      </c>
+      <c r="L39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" t="s">
+        <v>238</v>
+      </c>
+      <c r="G40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" t="s">
+        <v>238</v>
+      </c>
+      <c r="G41" t="s">
+        <v>239</v>
+      </c>
+      <c r="H41" t="s">
+        <v>239</v>
+      </c>
+      <c r="I41" t="s">
+        <v>239</v>
+      </c>
+      <c r="J41" t="s">
+        <v>239</v>
+      </c>
+      <c r="K41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>161</v>
+      </c>
+      <c r="H42" t="s">
+        <v>238</v>
+      </c>
+      <c r="I42" t="s">
+        <v>239</v>
+      </c>
+      <c r="J42" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>167</v>
+      </c>
+      <c r="J43" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F44" t="s">
+        <v>238</v>
+      </c>
+      <c r="G44" t="s">
+        <v>239</v>
+      </c>
+      <c r="H44" t="s">
+        <v>239</v>
+      </c>
+      <c r="I44" t="s">
+        <v>239</v>
+      </c>
+      <c r="J44" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" t="s">
+        <v>238</v>
+      </c>
+      <c r="J45" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="I46" t="s">
+        <v>238</v>
+      </c>
+      <c r="J46" t="s">
+        <v>239</v>
+      </c>
+      <c r="K46" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="J47" t="s">
+        <v>238</v>
+      </c>
+      <c r="K47" t="s">
+        <v>239</v>
+      </c>
+      <c r="L47" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="I48" t="s">
+        <v>238</v>
+      </c>
+      <c r="J48" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="H49" t="s">
+        <v>238</v>
+      </c>
+      <c r="I49" t="s">
+        <v>239</v>
+      </c>
+      <c r="J49" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC7FB74-2730-4C97-9F77-7A57F1B9797E}">
+  <dimension ref="A1:M31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>238</v>
+      </c>
+      <c r="H3" t="s">
+        <v>239</v>
+      </c>
+      <c r="I3" t="s">
+        <v>239</v>
+      </c>
+      <c r="J3" t="s">
+        <v>239</v>
+      </c>
+      <c r="K3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H4" t="s">
+        <v>239</v>
+      </c>
+      <c r="I4" t="s">
+        <v>239</v>
+      </c>
+      <c r="J4" t="s">
+        <v>239</v>
+      </c>
+      <c r="K4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>238</v>
+      </c>
+      <c r="I5" t="s">
+        <v>239</v>
+      </c>
+      <c r="J5" t="s">
+        <v>239</v>
+      </c>
+      <c r="K5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>238</v>
+      </c>
+      <c r="K6" t="s">
+        <v>239</v>
+      </c>
+      <c r="L6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>238</v>
+      </c>
+      <c r="H7" t="s">
+        <v>239</v>
+      </c>
+      <c r="I7" t="s">
+        <v>239</v>
+      </c>
+      <c r="J7" t="s">
+        <v>239</v>
+      </c>
+      <c r="K7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I8" t="s">
+        <v>239</v>
+      </c>
+      <c r="J8" t="s">
+        <v>239</v>
+      </c>
+      <c r="K8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>238</v>
+      </c>
+      <c r="I9" t="s">
+        <v>239</v>
+      </c>
+      <c r="J9" t="s">
+        <v>239</v>
+      </c>
+      <c r="K9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>270</v>
+      </c>
+      <c r="G10" t="s">
+        <v>238</v>
+      </c>
+      <c r="H10" t="s">
+        <v>239</v>
+      </c>
+      <c r="I10" t="s">
+        <v>239</v>
+      </c>
+      <c r="J10" t="s">
+        <v>239</v>
+      </c>
+      <c r="K10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" t="s">
+        <v>238</v>
+      </c>
+      <c r="J11" t="s">
+        <v>239</v>
+      </c>
+      <c r="K11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>238</v>
+      </c>
+      <c r="G12" t="s">
+        <v>239</v>
+      </c>
+      <c r="H12" t="s">
+        <v>239</v>
+      </c>
+      <c r="I12" t="s">
+        <v>239</v>
+      </c>
+      <c r="J12" t="s">
+        <v>239</v>
+      </c>
+      <c r="K12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>238</v>
+      </c>
+      <c r="H13" t="s">
+        <v>239</v>
+      </c>
+      <c r="I13" t="s">
+        <v>239</v>
+      </c>
+      <c r="J13" t="s">
+        <v>239</v>
+      </c>
+      <c r="K13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I14" t="s">
+        <v>239</v>
+      </c>
+      <c r="J14" t="s">
+        <v>239</v>
+      </c>
+      <c r="K14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>316</v>
+      </c>
+      <c r="F15" t="s">
+        <v>238</v>
+      </c>
+      <c r="G15" t="s">
+        <v>239</v>
+      </c>
+      <c r="H15" t="s">
+        <v>239</v>
+      </c>
+      <c r="I15" t="s">
+        <v>239</v>
+      </c>
+      <c r="J15" t="s">
+        <v>239</v>
+      </c>
+      <c r="K15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>238</v>
+      </c>
+      <c r="I16" t="s">
+        <v>239</v>
+      </c>
+      <c r="J16" t="s">
+        <v>239</v>
+      </c>
+      <c r="K16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>195</v>
+      </c>
+      <c r="F17" t="s">
+        <v>238</v>
+      </c>
+      <c r="G17" t="s">
+        <v>239</v>
+      </c>
+      <c r="H17" t="s">
+        <v>239</v>
+      </c>
+      <c r="I17" t="s">
+        <v>239</v>
+      </c>
+      <c r="J17" t="s">
+        <v>239</v>
+      </c>
+      <c r="K17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>238</v>
+      </c>
+      <c r="G18" t="s">
+        <v>239</v>
+      </c>
+      <c r="H18" t="s">
+        <v>239</v>
+      </c>
+      <c r="I18" t="s">
+        <v>239</v>
+      </c>
+      <c r="J18" t="s">
+        <v>239</v>
+      </c>
+      <c r="K18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>93</v>
+      </c>
+      <c r="J19" t="s">
+        <v>238</v>
+      </c>
+      <c r="K19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>158</v>
+      </c>
+      <c r="H20" t="s">
+        <v>238</v>
+      </c>
+      <c r="I20" t="s">
+        <v>239</v>
+      </c>
+      <c r="J20" t="s">
+        <v>239</v>
+      </c>
+      <c r="K20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>232</v>
+      </c>
+      <c r="H21" t="s">
+        <v>238</v>
+      </c>
+      <c r="I21" t="s">
+        <v>239</v>
+      </c>
+      <c r="J21" t="s">
+        <v>239</v>
+      </c>
+      <c r="K21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>235</v>
+      </c>
+      <c r="H22" t="s">
+        <v>238</v>
+      </c>
+      <c r="I22" t="s">
+        <v>239</v>
+      </c>
+      <c r="J22" t="s">
+        <v>239</v>
+      </c>
+      <c r="K22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" t="s">
+        <v>238</v>
+      </c>
+      <c r="I23" t="s">
+        <v>239</v>
+      </c>
+      <c r="J23" t="s">
+        <v>239</v>
+      </c>
+      <c r="K23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" t="s">
+        <v>238</v>
+      </c>
+      <c r="K24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
+        <v>238</v>
+      </c>
+      <c r="G25" t="s">
+        <v>239</v>
+      </c>
+      <c r="H25" t="s">
+        <v>239</v>
+      </c>
+      <c r="I25" t="s">
+        <v>239</v>
+      </c>
+      <c r="J25" t="s">
+        <v>239</v>
+      </c>
+      <c r="K25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>238</v>
+      </c>
+      <c r="G26" t="s">
+        <v>239</v>
+      </c>
+      <c r="H26" t="s">
+        <v>239</v>
+      </c>
+      <c r="I26" t="s">
+        <v>239</v>
+      </c>
+      <c r="J26" t="s">
+        <v>239</v>
+      </c>
+      <c r="K26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" t="s">
+        <v>238</v>
+      </c>
+      <c r="J27" t="s">
+        <v>239</v>
+      </c>
+      <c r="K27" t="s">
+        <v>239</v>
+      </c>
+      <c r="L27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="H28" t="s">
+        <v>238</v>
+      </c>
+      <c r="I28" t="s">
+        <v>239</v>
+      </c>
+      <c r="J28" t="s">
+        <v>239</v>
+      </c>
+      <c r="K28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>311</v>
+      </c>
+      <c r="F29" t="s">
+        <v>238</v>
+      </c>
+      <c r="G29" t="s">
+        <v>239</v>
+      </c>
+      <c r="H29" t="s">
+        <v>239</v>
+      </c>
+      <c r="I29" t="s">
+        <v>239</v>
+      </c>
+      <c r="J29" t="s">
+        <v>239</v>
+      </c>
+      <c r="K29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>49</v>
+      </c>
+      <c r="J30" t="s">
+        <v>238</v>
+      </c>
+      <c r="K30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="J31" t="s">
+        <v>238</v>
+      </c>
+      <c r="K31" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a few more states and sources.
</commit_message>
<xml_diff>
--- a/data/raw/State_Sources.xlsx
+++ b/data/raw/State_Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chigham\Documents\forkranger-us-regions\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963C7F03-68E1-4DE3-9FA7-2B0BE110835C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3180CE0A-A51F-40BA-8BA6-E39DDAD066B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="26" activeTab="35" xr2:uid="{1A035CB0-260D-4ABF-9F3B-5033D39FF1A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="33" activeTab="42" xr2:uid="{1A035CB0-260D-4ABF-9F3B-5033D39FF1A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Alabama" sheetId="1" r:id="rId1"/>
@@ -49,6 +49,13 @@
     <sheet name="North Carolina" sheetId="34" r:id="rId34"/>
     <sheet name="North Dakota" sheetId="35" r:id="rId35"/>
     <sheet name="Ohio" sheetId="36" r:id="rId36"/>
+    <sheet name="Oklahoma" sheetId="37" r:id="rId37"/>
+    <sheet name="Oregon" sheetId="38" r:id="rId38"/>
+    <sheet name="Pennsylvania" sheetId="39" r:id="rId39"/>
+    <sheet name="Puerto Rico" sheetId="40" r:id="rId40"/>
+    <sheet name="Rhode Island" sheetId="41" r:id="rId41"/>
+    <sheet name="South Carolina" sheetId="42" r:id="rId42"/>
+    <sheet name="South Dakota" sheetId="43" r:id="rId43"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8061" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9387" uniqueCount="383">
   <si>
     <t>Greens (Collards, turnips, etc.)</t>
   </si>
@@ -1124,6 +1131,102 @@
   </si>
   <si>
     <t>Meskmelon</t>
+  </si>
+  <si>
+    <t>Blackeye Peas</t>
+  </si>
+  <si>
+    <t>Tomatoes Green</t>
+  </si>
+  <si>
+    <t>Tomatoes Red</t>
+  </si>
+  <si>
+    <t>Mixed Greens</t>
+  </si>
+  <si>
+    <t>Pawpaw</t>
+  </si>
+  <si>
+    <t>Squash Winter</t>
+  </si>
+  <si>
+    <t>Squash Summer</t>
+  </si>
+  <si>
+    <t>Acerola</t>
+  </si>
+  <si>
+    <t>Sweet Pepper</t>
+  </si>
+  <si>
+    <t>Star Fruit</t>
+  </si>
+  <si>
+    <t>Coconut</t>
+  </si>
+  <si>
+    <t>Custards Apple</t>
+  </si>
+  <si>
+    <t>Pigeon Peas</t>
+  </si>
+  <si>
+    <t>Soursop</t>
+  </si>
+  <si>
+    <t>Lemon</t>
+  </si>
+  <si>
+    <t>Cocoyam</t>
+  </si>
+  <si>
+    <t>Mamey</t>
+  </si>
+  <si>
+    <t>Sapote Mamey</t>
+  </si>
+  <si>
+    <t>Mandarines</t>
+  </si>
+  <si>
+    <t>Flowery Yam</t>
+  </si>
+  <si>
+    <t>Habanero Yam</t>
+  </si>
+  <si>
+    <t>Medlar</t>
+  </si>
+  <si>
+    <t>Plantain</t>
+  </si>
+  <si>
+    <t>Tamarind</t>
+  </si>
+  <si>
+    <t>Pink Grapefruit</t>
+  </si>
+  <si>
+    <t>White Taro</t>
+  </si>
+  <si>
+    <t>Purple Taro</t>
+  </si>
+  <si>
+    <t>Cassava</t>
+  </si>
+  <si>
+    <t>Breadfruit</t>
+  </si>
+  <si>
+    <t>Honeydew Melon</t>
+  </si>
+  <si>
+    <t>Limes</t>
+  </si>
+  <si>
+    <t>Pineapples</t>
   </si>
 </sst>
 </file>
@@ -19369,7 +19472,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22392,7 +22495,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC7FB74-2730-4C97-9F77-7A57F1B9797E}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -22977,6 +23082,1592 @@
         <v>238</v>
       </c>
       <c r="K31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A36A21-2118-4F7C-8C75-9D2A75AA3523}">
+  <dimension ref="A1:M41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>238</v>
+      </c>
+      <c r="F3" t="s">
+        <v>239</v>
+      </c>
+      <c r="G3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G4" t="s">
+        <v>237</v>
+      </c>
+      <c r="J4" t="s">
+        <v>238</v>
+      </c>
+      <c r="K4" t="s">
+        <v>239</v>
+      </c>
+      <c r="L4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H5" t="s">
+        <v>239</v>
+      </c>
+      <c r="I5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>351</v>
+      </c>
+      <c r="H6" t="s">
+        <v>238</v>
+      </c>
+      <c r="I6" t="s">
+        <v>239</v>
+      </c>
+      <c r="J6" t="s">
+        <v>239</v>
+      </c>
+      <c r="K6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>238</v>
+      </c>
+      <c r="H7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>238</v>
+      </c>
+      <c r="F8" t="s">
+        <v>239</v>
+      </c>
+      <c r="G8" t="s">
+        <v>237</v>
+      </c>
+      <c r="J8" t="s">
+        <v>238</v>
+      </c>
+      <c r="K8" t="s">
+        <v>239</v>
+      </c>
+      <c r="L8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>238</v>
+      </c>
+      <c r="G9" t="s">
+        <v>239</v>
+      </c>
+      <c r="H9" t="s">
+        <v>237</v>
+      </c>
+      <c r="J9" t="s">
+        <v>238</v>
+      </c>
+      <c r="K9" t="s">
+        <v>239</v>
+      </c>
+      <c r="L9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" t="s">
+        <v>238</v>
+      </c>
+      <c r="I10" t="s">
+        <v>237</v>
+      </c>
+      <c r="J10" t="s">
+        <v>239</v>
+      </c>
+      <c r="K10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F11" t="s">
+        <v>239</v>
+      </c>
+      <c r="G11" t="s">
+        <v>237</v>
+      </c>
+      <c r="J11" t="s">
+        <v>238</v>
+      </c>
+      <c r="K11" t="s">
+        <v>239</v>
+      </c>
+      <c r="L11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>238</v>
+      </c>
+      <c r="G12" t="s">
+        <v>237</v>
+      </c>
+      <c r="J12" t="s">
+        <v>238</v>
+      </c>
+      <c r="K12" t="s">
+        <v>239</v>
+      </c>
+      <c r="L12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" t="s">
+        <v>238</v>
+      </c>
+      <c r="H13" t="s">
+        <v>239</v>
+      </c>
+      <c r="I13" t="s">
+        <v>239</v>
+      </c>
+      <c r="J13" t="s">
+        <v>239</v>
+      </c>
+      <c r="K13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I14" t="s">
+        <v>239</v>
+      </c>
+      <c r="J14" t="s">
+        <v>239</v>
+      </c>
+      <c r="K14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" t="s">
+        <v>238</v>
+      </c>
+      <c r="H15" t="s">
+        <v>239</v>
+      </c>
+      <c r="I15" t="s">
+        <v>239</v>
+      </c>
+      <c r="J15" t="s">
+        <v>239</v>
+      </c>
+      <c r="K15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" t="s">
+        <v>238</v>
+      </c>
+      <c r="G16" t="s">
+        <v>239</v>
+      </c>
+      <c r="H16" t="s">
+        <v>237</v>
+      </c>
+      <c r="J16" t="s">
+        <v>238</v>
+      </c>
+      <c r="K16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>177</v>
+      </c>
+      <c r="E17" t="s">
+        <v>238</v>
+      </c>
+      <c r="F17" t="s">
+        <v>237</v>
+      </c>
+      <c r="J17" t="s">
+        <v>238</v>
+      </c>
+      <c r="K17" t="s">
+        <v>239</v>
+      </c>
+      <c r="L17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>238</v>
+      </c>
+      <c r="F18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G18" t="s">
+        <v>239</v>
+      </c>
+      <c r="H18" t="s">
+        <v>239</v>
+      </c>
+      <c r="I18" t="s">
+        <v>239</v>
+      </c>
+      <c r="J18" t="s">
+        <v>239</v>
+      </c>
+      <c r="K18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>238</v>
+      </c>
+      <c r="F19" t="s">
+        <v>239</v>
+      </c>
+      <c r="G19" t="s">
+        <v>237</v>
+      </c>
+      <c r="J19" t="s">
+        <v>238</v>
+      </c>
+      <c r="K19" t="s">
+        <v>239</v>
+      </c>
+      <c r="L19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
+        <v>238</v>
+      </c>
+      <c r="I20" t="s">
+        <v>239</v>
+      </c>
+      <c r="J20" t="s">
+        <v>239</v>
+      </c>
+      <c r="K20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>238</v>
+      </c>
+      <c r="F21" t="s">
+        <v>239</v>
+      </c>
+      <c r="G21" t="s">
+        <v>239</v>
+      </c>
+      <c r="H21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" t="s">
+        <v>238</v>
+      </c>
+      <c r="H22" t="s">
+        <v>239</v>
+      </c>
+      <c r="I22" t="s">
+        <v>239</v>
+      </c>
+      <c r="J22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" t="s">
+        <v>238</v>
+      </c>
+      <c r="J23" t="s">
+        <v>239</v>
+      </c>
+      <c r="K23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="s">
+        <v>238</v>
+      </c>
+      <c r="F24" t="s">
+        <v>237</v>
+      </c>
+      <c r="J24" t="s">
+        <v>238</v>
+      </c>
+      <c r="K24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>176</v>
+      </c>
+      <c r="E25" t="s">
+        <v>238</v>
+      </c>
+      <c r="F25" t="s">
+        <v>237</v>
+      </c>
+      <c r="J25" t="s">
+        <v>238</v>
+      </c>
+      <c r="K25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" t="s">
+        <v>238</v>
+      </c>
+      <c r="I26" t="s">
+        <v>239</v>
+      </c>
+      <c r="J26" t="s">
+        <v>239</v>
+      </c>
+      <c r="K26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>238</v>
+      </c>
+      <c r="G27" t="s">
+        <v>239</v>
+      </c>
+      <c r="H27" t="s">
+        <v>239</v>
+      </c>
+      <c r="I27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" t="s">
+        <v>238</v>
+      </c>
+      <c r="J28" t="s">
+        <v>239</v>
+      </c>
+      <c r="K28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>238</v>
+      </c>
+      <c r="E29" t="s">
+        <v>239</v>
+      </c>
+      <c r="F29" t="s">
+        <v>237</v>
+      </c>
+      <c r="J29" t="s">
+        <v>238</v>
+      </c>
+      <c r="K29" t="s">
+        <v>239</v>
+      </c>
+      <c r="L29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" t="s">
+        <v>238</v>
+      </c>
+      <c r="H30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>238</v>
+      </c>
+      <c r="E31" t="s">
+        <v>239</v>
+      </c>
+      <c r="F31" t="s">
+        <v>239</v>
+      </c>
+      <c r="G31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>238</v>
+      </c>
+      <c r="E32" t="s">
+        <v>239</v>
+      </c>
+      <c r="F32" t="s">
+        <v>239</v>
+      </c>
+      <c r="G32" t="s">
+        <v>237</v>
+      </c>
+      <c r="J32" t="s">
+        <v>238</v>
+      </c>
+      <c r="K32" t="s">
+        <v>239</v>
+      </c>
+      <c r="L32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>161</v>
+      </c>
+      <c r="F33" t="s">
+        <v>238</v>
+      </c>
+      <c r="G33" t="s">
+        <v>239</v>
+      </c>
+      <c r="H33" t="s">
+        <v>239</v>
+      </c>
+      <c r="I33" t="s">
+        <v>239</v>
+      </c>
+      <c r="J33" t="s">
+        <v>239</v>
+      </c>
+      <c r="K33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>238</v>
+      </c>
+      <c r="G34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35" t="s">
+        <v>238</v>
+      </c>
+      <c r="H35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>167</v>
+      </c>
+      <c r="J36" t="s">
+        <v>238</v>
+      </c>
+      <c r="K36" t="s">
+        <v>239</v>
+      </c>
+      <c r="L36" t="s">
+        <v>239</v>
+      </c>
+      <c r="M36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>352</v>
+      </c>
+      <c r="F37" t="s">
+        <v>238</v>
+      </c>
+      <c r="G37" t="s">
+        <v>239</v>
+      </c>
+      <c r="H37" t="s">
+        <v>239</v>
+      </c>
+      <c r="I37" t="s">
+        <v>239</v>
+      </c>
+      <c r="J37" t="s">
+        <v>239</v>
+      </c>
+      <c r="K37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>353</v>
+      </c>
+      <c r="F38" t="s">
+        <v>238</v>
+      </c>
+      <c r="G38" t="s">
+        <v>239</v>
+      </c>
+      <c r="H38" t="s">
+        <v>239</v>
+      </c>
+      <c r="I38" t="s">
+        <v>239</v>
+      </c>
+      <c r="J38" t="s">
+        <v>239</v>
+      </c>
+      <c r="K38" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" t="s">
+        <v>238</v>
+      </c>
+      <c r="E39" t="s">
+        <v>239</v>
+      </c>
+      <c r="F39" t="s">
+        <v>239</v>
+      </c>
+      <c r="G39" t="s">
+        <v>237</v>
+      </c>
+      <c r="J39" t="s">
+        <v>238</v>
+      </c>
+      <c r="K39" t="s">
+        <v>239</v>
+      </c>
+      <c r="L39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>127</v>
+      </c>
+      <c r="H40" t="s">
+        <v>238</v>
+      </c>
+      <c r="I40" t="s">
+        <v>239</v>
+      </c>
+      <c r="J40" t="s">
+        <v>239</v>
+      </c>
+      <c r="K40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="H41" t="s">
+        <v>238</v>
+      </c>
+      <c r="I41" t="s">
+        <v>239</v>
+      </c>
+      <c r="J41" t="s">
+        <v>239</v>
+      </c>
+      <c r="K41" t="s">
+        <v>239</v>
+      </c>
+      <c r="L41" t="s">
+        <v>239</v>
+      </c>
+      <c r="M41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2961229-E5B0-4B6D-A4E0-45B1DC3465AC}">
+  <dimension ref="B1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679A2919-020B-4253-9BEF-E2E16A6FC39C}">
+  <dimension ref="A1:M40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" t="s">
+        <v>338</v>
+      </c>
+      <c r="H2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K2" t="s">
+        <v>237</v>
+      </c>
+      <c r="L2" t="s">
+        <v>338</v>
+      </c>
+      <c r="M2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I4" t="s">
+        <v>239</v>
+      </c>
+      <c r="J4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>238</v>
+      </c>
+      <c r="I5" t="s">
+        <v>239</v>
+      </c>
+      <c r="J5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>238</v>
+      </c>
+      <c r="I6" t="s">
+        <v>239</v>
+      </c>
+      <c r="J6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>238</v>
+      </c>
+      <c r="I7" t="s">
+        <v>239</v>
+      </c>
+      <c r="J7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G8" t="s">
+        <v>237</v>
+      </c>
+      <c r="K8" t="s">
+        <v>238</v>
+      </c>
+      <c r="L8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>238</v>
+      </c>
+      <c r="H9" t="s">
+        <v>237</v>
+      </c>
+      <c r="J9" t="s">
+        <v>238</v>
+      </c>
+      <c r="K9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="I10" t="s">
+        <v>238</v>
+      </c>
+      <c r="J10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s">
+        <v>238</v>
+      </c>
+      <c r="I11" t="s">
+        <v>239</v>
+      </c>
+      <c r="J11" t="s">
+        <v>239</v>
+      </c>
+      <c r="K11" t="s">
+        <v>237</v>
+      </c>
+      <c r="L11" t="s">
+        <v>338</v>
+      </c>
+      <c r="M11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>238</v>
+      </c>
+      <c r="H12" t="s">
+        <v>237</v>
+      </c>
+      <c r="K12" t="s">
+        <v>238</v>
+      </c>
+      <c r="L12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>238</v>
+      </c>
+      <c r="H13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I14" t="s">
+        <v>239</v>
+      </c>
+      <c r="J14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" t="s">
+        <v>238</v>
+      </c>
+      <c r="I15" t="s">
+        <v>239</v>
+      </c>
+      <c r="J15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>238</v>
+      </c>
+      <c r="I16" t="s">
+        <v>239</v>
+      </c>
+      <c r="J16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="I17" t="s">
+        <v>238</v>
+      </c>
+      <c r="J17" t="s">
+        <v>239</v>
+      </c>
+      <c r="K17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" t="s">
+        <v>238</v>
+      </c>
+      <c r="H18" t="s">
+        <v>239</v>
+      </c>
+      <c r="I18" t="s">
+        <v>239</v>
+      </c>
+      <c r="J18" t="s">
+        <v>239</v>
+      </c>
+      <c r="K18" t="s">
+        <v>239</v>
+      </c>
+      <c r="L18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>354</v>
+      </c>
+      <c r="E19" t="s">
+        <v>238</v>
+      </c>
+      <c r="F19" t="s">
+        <v>237</v>
+      </c>
+      <c r="I19" t="s">
+        <v>238</v>
+      </c>
+      <c r="J19" t="s">
+        <v>239</v>
+      </c>
+      <c r="K19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" t="s">
+        <v>239</v>
+      </c>
+      <c r="C20" t="s">
+        <v>239</v>
+      </c>
+      <c r="D20" t="s">
+        <v>239</v>
+      </c>
+      <c r="E20" t="s">
+        <v>239</v>
+      </c>
+      <c r="F20" t="s">
+        <v>239</v>
+      </c>
+      <c r="G20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H20" t="s">
+        <v>239</v>
+      </c>
+      <c r="I20" t="s">
+        <v>239</v>
+      </c>
+      <c r="J20" t="s">
+        <v>239</v>
+      </c>
+      <c r="K20" t="s">
+        <v>239</v>
+      </c>
+      <c r="L20" t="s">
+        <v>239</v>
+      </c>
+      <c r="M20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>168</v>
+      </c>
+      <c r="H21" t="s">
+        <v>238</v>
+      </c>
+      <c r="I21" t="s">
+        <v>239</v>
+      </c>
+      <c r="J21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" t="s">
+        <v>238</v>
+      </c>
+      <c r="I22" t="s">
+        <v>239</v>
+      </c>
+      <c r="J22" t="s">
+        <v>239</v>
+      </c>
+      <c r="K22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>355</v>
+      </c>
+      <c r="J23" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" t="s">
+        <v>238</v>
+      </c>
+      <c r="I24" t="s">
+        <v>239</v>
+      </c>
+      <c r="J24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="I25" t="s">
+        <v>238</v>
+      </c>
+      <c r="J25" t="s">
+        <v>239</v>
+      </c>
+      <c r="K25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" t="s">
+        <v>238</v>
+      </c>
+      <c r="G26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>238</v>
+      </c>
+      <c r="I27" t="s">
+        <v>239</v>
+      </c>
+      <c r="J27" t="s">
+        <v>239</v>
+      </c>
+      <c r="K27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" t="s">
+        <v>238</v>
+      </c>
+      <c r="J28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>338</v>
+      </c>
+      <c r="H29" t="s">
+        <v>238</v>
+      </c>
+      <c r="I29" t="s">
+        <v>239</v>
+      </c>
+      <c r="J29" t="s">
+        <v>237</v>
+      </c>
+      <c r="K29" t="s">
+        <v>338</v>
+      </c>
+      <c r="L29" t="s">
+        <v>338</v>
+      </c>
+      <c r="M29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" t="s">
+        <v>238</v>
+      </c>
+      <c r="K30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" t="s">
+        <v>238</v>
+      </c>
+      <c r="G31" t="s">
+        <v>237</v>
+      </c>
+      <c r="J31" t="s">
+        <v>238</v>
+      </c>
+      <c r="K31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="H32" t="s">
+        <v>238</v>
+      </c>
+      <c r="I32" t="s">
+        <v>239</v>
+      </c>
+      <c r="J32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
+        <v>238</v>
+      </c>
+      <c r="G33" t="s">
+        <v>237</v>
+      </c>
+      <c r="J33" t="s">
+        <v>238</v>
+      </c>
+      <c r="K33" t="s">
+        <v>239</v>
+      </c>
+      <c r="L33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>357</v>
+      </c>
+      <c r="G34" t="s">
+        <v>238</v>
+      </c>
+      <c r="H34" t="s">
+        <v>239</v>
+      </c>
+      <c r="I34" t="s">
+        <v>239</v>
+      </c>
+      <c r="J34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>356</v>
+      </c>
+      <c r="B35" t="s">
+        <v>338</v>
+      </c>
+      <c r="C35" t="s">
+        <v>338</v>
+      </c>
+      <c r="I35" t="s">
+        <v>238</v>
+      </c>
+      <c r="J35" t="s">
+        <v>239</v>
+      </c>
+      <c r="K35" t="s">
+        <v>237</v>
+      </c>
+      <c r="L35" t="s">
+        <v>338</v>
+      </c>
+      <c r="M35" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>167</v>
+      </c>
+      <c r="B37" t="s">
+        <v>338</v>
+      </c>
+      <c r="C37" t="s">
+        <v>338</v>
+      </c>
+      <c r="J37" t="s">
+        <v>238</v>
+      </c>
+      <c r="K37" t="s">
+        <v>237</v>
+      </c>
+      <c r="L37" t="s">
+        <v>338</v>
+      </c>
+      <c r="M37" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H38" t="s">
+        <v>238</v>
+      </c>
+      <c r="I38" t="s">
+        <v>239</v>
+      </c>
+      <c r="J38" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" t="s">
+        <v>238</v>
+      </c>
+      <c r="F39" t="s">
+        <v>237</v>
+      </c>
+      <c r="J39" t="s">
+        <v>238</v>
+      </c>
+      <c r="K39" t="s">
+        <v>239</v>
+      </c>
+      <c r="L39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>127</v>
+      </c>
+      <c r="H40" t="s">
+        <v>238</v>
+      </c>
+      <c r="I40" t="s">
         <v>237</v>
       </c>
     </row>
@@ -24089,6 +25780,2931 @@
         <v>239</v>
       </c>
       <c r="M47" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E81C2A9-D250-4D1C-9235-C36A4FD70631}">
+  <dimension ref="A1:M48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G2" t="s">
+        <v>239</v>
+      </c>
+      <c r="H2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L2" t="s">
+        <v>239</v>
+      </c>
+      <c r="M2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F3" t="s">
+        <v>239</v>
+      </c>
+      <c r="G3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H3" t="s">
+        <v>239</v>
+      </c>
+      <c r="I3" t="s">
+        <v>239</v>
+      </c>
+      <c r="J3" t="s">
+        <v>239</v>
+      </c>
+      <c r="K3" t="s">
+        <v>239</v>
+      </c>
+      <c r="L3" t="s">
+        <v>239</v>
+      </c>
+      <c r="M3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>359</v>
+      </c>
+      <c r="F4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H4" t="s">
+        <v>239</v>
+      </c>
+      <c r="I4" t="s">
+        <v>239</v>
+      </c>
+      <c r="J4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E5" t="s">
+        <v>237</v>
+      </c>
+      <c r="L5" t="s">
+        <v>238</v>
+      </c>
+      <c r="M5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F6" t="s">
+        <v>239</v>
+      </c>
+      <c r="G6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>238</v>
+      </c>
+      <c r="H7" t="s">
+        <v>239</v>
+      </c>
+      <c r="I7" t="s">
+        <v>239</v>
+      </c>
+      <c r="J7" t="s">
+        <v>239</v>
+      </c>
+      <c r="K7" t="s">
+        <v>239</v>
+      </c>
+      <c r="L7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E8" t="s">
+        <v>239</v>
+      </c>
+      <c r="F8" t="s">
+        <v>239</v>
+      </c>
+      <c r="G8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I8" t="s">
+        <v>239</v>
+      </c>
+      <c r="J8" t="s">
+        <v>239</v>
+      </c>
+      <c r="K8" t="s">
+        <v>239</v>
+      </c>
+      <c r="L8" t="s">
+        <v>239</v>
+      </c>
+      <c r="M8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>360</v>
+      </c>
+      <c r="D9" t="s">
+        <v>238</v>
+      </c>
+      <c r="E9" t="s">
+        <v>239</v>
+      </c>
+      <c r="F9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G9" t="s">
+        <v>239</v>
+      </c>
+      <c r="H9" t="s">
+        <v>239</v>
+      </c>
+      <c r="I9" t="s">
+        <v>239</v>
+      </c>
+      <c r="J9" t="s">
+        <v>239</v>
+      </c>
+      <c r="K9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" t="s">
+        <v>239</v>
+      </c>
+      <c r="E10" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" t="s">
+        <v>239</v>
+      </c>
+      <c r="G10" t="s">
+        <v>237</v>
+      </c>
+      <c r="M10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>361</v>
+      </c>
+      <c r="B11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" t="s">
+        <v>239</v>
+      </c>
+      <c r="E11" t="s">
+        <v>239</v>
+      </c>
+      <c r="F11" t="s">
+        <v>239</v>
+      </c>
+      <c r="G11" t="s">
+        <v>239</v>
+      </c>
+      <c r="H11" t="s">
+        <v>239</v>
+      </c>
+      <c r="I11" t="s">
+        <v>239</v>
+      </c>
+      <c r="J11" t="s">
+        <v>239</v>
+      </c>
+      <c r="K11" t="s">
+        <v>239</v>
+      </c>
+      <c r="L11" t="s">
+        <v>239</v>
+      </c>
+      <c r="M11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>362</v>
+      </c>
+      <c r="C12" t="s">
+        <v>238</v>
+      </c>
+      <c r="D12" t="s">
+        <v>239</v>
+      </c>
+      <c r="E12" t="s">
+        <v>239</v>
+      </c>
+      <c r="F12" t="s">
+        <v>239</v>
+      </c>
+      <c r="G12" t="s">
+        <v>239</v>
+      </c>
+      <c r="H12" t="s">
+        <v>239</v>
+      </c>
+      <c r="I12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C13" t="s">
+        <v>237</v>
+      </c>
+      <c r="K13" t="s">
+        <v>238</v>
+      </c>
+      <c r="L13" t="s">
+        <v>239</v>
+      </c>
+      <c r="M13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D14" t="s">
+        <v>239</v>
+      </c>
+      <c r="E14" t="s">
+        <v>239</v>
+      </c>
+      <c r="F14" t="s">
+        <v>239</v>
+      </c>
+      <c r="G14" t="s">
+        <v>239</v>
+      </c>
+      <c r="H14" t="s">
+        <v>239</v>
+      </c>
+      <c r="I14" t="s">
+        <v>239</v>
+      </c>
+      <c r="J14" t="s">
+        <v>239</v>
+      </c>
+      <c r="K14" t="s">
+        <v>239</v>
+      </c>
+      <c r="L14" t="s">
+        <v>239</v>
+      </c>
+      <c r="M14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>238</v>
+      </c>
+      <c r="E15" t="s">
+        <v>239</v>
+      </c>
+      <c r="F15" t="s">
+        <v>239</v>
+      </c>
+      <c r="G15" t="s">
+        <v>239</v>
+      </c>
+      <c r="H15" t="s">
+        <v>239</v>
+      </c>
+      <c r="I15" t="s">
+        <v>239</v>
+      </c>
+      <c r="J15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>363</v>
+      </c>
+      <c r="B16" t="s">
+        <v>239</v>
+      </c>
+      <c r="C16" t="s">
+        <v>237</v>
+      </c>
+      <c r="K16" t="s">
+        <v>238</v>
+      </c>
+      <c r="L16" t="s">
+        <v>239</v>
+      </c>
+      <c r="M16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>364</v>
+      </c>
+      <c r="C17" t="s">
+        <v>238</v>
+      </c>
+      <c r="D17" t="s">
+        <v>237</v>
+      </c>
+      <c r="H17" t="s">
+        <v>238</v>
+      </c>
+      <c r="I17" t="s">
+        <v>239</v>
+      </c>
+      <c r="J17" t="s">
+        <v>239</v>
+      </c>
+      <c r="K17" t="s">
+        <v>239</v>
+      </c>
+      <c r="L17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C18" t="s">
+        <v>239</v>
+      </c>
+      <c r="D18" t="s">
+        <v>239</v>
+      </c>
+      <c r="E18" t="s">
+        <v>239</v>
+      </c>
+      <c r="F18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G18" t="s">
+        <v>239</v>
+      </c>
+      <c r="H18" t="s">
+        <v>239</v>
+      </c>
+      <c r="I18" t="s">
+        <v>239</v>
+      </c>
+      <c r="J18" t="s">
+        <v>239</v>
+      </c>
+      <c r="K18" t="s">
+        <v>239</v>
+      </c>
+      <c r="L18" t="s">
+        <v>239</v>
+      </c>
+      <c r="M18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19" t="s">
+        <v>239</v>
+      </c>
+      <c r="D19" t="s">
+        <v>239</v>
+      </c>
+      <c r="E19" t="s">
+        <v>239</v>
+      </c>
+      <c r="F19" t="s">
+        <v>239</v>
+      </c>
+      <c r="G19" t="s">
+        <v>237</v>
+      </c>
+      <c r="L19" t="s">
+        <v>238</v>
+      </c>
+      <c r="M19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" t="s">
+        <v>239</v>
+      </c>
+      <c r="C20" t="s">
+        <v>239</v>
+      </c>
+      <c r="D20" t="s">
+        <v>239</v>
+      </c>
+      <c r="E20" t="s">
+        <v>239</v>
+      </c>
+      <c r="F20" t="s">
+        <v>237</v>
+      </c>
+      <c r="L20" t="s">
+        <v>238</v>
+      </c>
+      <c r="M20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" t="s">
+        <v>239</v>
+      </c>
+      <c r="D21" t="s">
+        <v>239</v>
+      </c>
+      <c r="E21" t="s">
+        <v>239</v>
+      </c>
+      <c r="F21" t="s">
+        <v>237</v>
+      </c>
+      <c r="I21" t="s">
+        <v>238</v>
+      </c>
+      <c r="J21" t="s">
+        <v>239</v>
+      </c>
+      <c r="K21" t="s">
+        <v>239</v>
+      </c>
+      <c r="L21" t="s">
+        <v>239</v>
+      </c>
+      <c r="M21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" t="s">
+        <v>239</v>
+      </c>
+      <c r="C22" t="s">
+        <v>239</v>
+      </c>
+      <c r="D22" t="s">
+        <v>239</v>
+      </c>
+      <c r="E22" t="s">
+        <v>239</v>
+      </c>
+      <c r="F22" t="s">
+        <v>239</v>
+      </c>
+      <c r="G22" t="s">
+        <v>239</v>
+      </c>
+      <c r="H22" t="s">
+        <v>239</v>
+      </c>
+      <c r="I22" t="s">
+        <v>239</v>
+      </c>
+      <c r="J22" t="s">
+        <v>239</v>
+      </c>
+      <c r="K22" t="s">
+        <v>239</v>
+      </c>
+      <c r="L22" t="s">
+        <v>239</v>
+      </c>
+      <c r="M22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>365</v>
+      </c>
+      <c r="B23" t="s">
+        <v>239</v>
+      </c>
+      <c r="C23" t="s">
+        <v>239</v>
+      </c>
+      <c r="D23" t="s">
+        <v>239</v>
+      </c>
+      <c r="E23" t="s">
+        <v>239</v>
+      </c>
+      <c r="F23" t="s">
+        <v>239</v>
+      </c>
+      <c r="G23" t="s">
+        <v>237</v>
+      </c>
+      <c r="L23" t="s">
+        <v>238</v>
+      </c>
+      <c r="M23" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" t="s">
+        <v>239</v>
+      </c>
+      <c r="D24" t="s">
+        <v>237</v>
+      </c>
+      <c r="L24" t="s">
+        <v>238</v>
+      </c>
+      <c r="M24" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>366</v>
+      </c>
+      <c r="C25" t="s">
+        <v>238</v>
+      </c>
+      <c r="D25" t="s">
+        <v>239</v>
+      </c>
+      <c r="E25" t="s">
+        <v>239</v>
+      </c>
+      <c r="F25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>367</v>
+      </c>
+      <c r="D26" t="s">
+        <v>238</v>
+      </c>
+      <c r="E26" t="s">
+        <v>239</v>
+      </c>
+      <c r="F26" t="s">
+        <v>239</v>
+      </c>
+      <c r="G26" t="s">
+        <v>239</v>
+      </c>
+      <c r="H26" t="s">
+        <v>239</v>
+      </c>
+      <c r="I26" t="s">
+        <v>239</v>
+      </c>
+      <c r="J26" t="s">
+        <v>239</v>
+      </c>
+      <c r="K26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>368</v>
+      </c>
+      <c r="C27" t="s">
+        <v>238</v>
+      </c>
+      <c r="D27" t="s">
+        <v>239</v>
+      </c>
+      <c r="E27" t="s">
+        <v>239</v>
+      </c>
+      <c r="F27" t="s">
+        <v>239</v>
+      </c>
+      <c r="G27" t="s">
+        <v>239</v>
+      </c>
+      <c r="H27" t="s">
+        <v>239</v>
+      </c>
+      <c r="I27" t="s">
+        <v>239</v>
+      </c>
+      <c r="J27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>369</v>
+      </c>
+      <c r="B28" t="s">
+        <v>239</v>
+      </c>
+      <c r="C28" t="s">
+        <v>239</v>
+      </c>
+      <c r="D28" t="s">
+        <v>239</v>
+      </c>
+      <c r="E28" t="s">
+        <v>237</v>
+      </c>
+      <c r="J28" t="s">
+        <v>238</v>
+      </c>
+      <c r="K28" t="s">
+        <v>239</v>
+      </c>
+      <c r="L28" t="s">
+        <v>239</v>
+      </c>
+      <c r="M28" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>184</v>
+      </c>
+      <c r="F29" t="s">
+        <v>238</v>
+      </c>
+      <c r="G29" t="s">
+        <v>239</v>
+      </c>
+      <c r="H29" t="s">
+        <v>239</v>
+      </c>
+      <c r="I29" t="s">
+        <v>239</v>
+      </c>
+      <c r="J29" t="s">
+        <v>239</v>
+      </c>
+      <c r="K29" t="s">
+        <v>239</v>
+      </c>
+      <c r="L29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F30" t="s">
+        <v>238</v>
+      </c>
+      <c r="G30" t="s">
+        <v>239</v>
+      </c>
+      <c r="H30" t="s">
+        <v>239</v>
+      </c>
+      <c r="I30" t="s">
+        <v>239</v>
+      </c>
+      <c r="J30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>370</v>
+      </c>
+      <c r="C31" t="s">
+        <v>238</v>
+      </c>
+      <c r="D31" t="s">
+        <v>239</v>
+      </c>
+      <c r="E31" t="s">
+        <v>239</v>
+      </c>
+      <c r="F31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>371</v>
+      </c>
+      <c r="H32" t="s">
+        <v>238</v>
+      </c>
+      <c r="I32" t="s">
+        <v>239</v>
+      </c>
+      <c r="J32" t="s">
+        <v>239</v>
+      </c>
+      <c r="K32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>372</v>
+      </c>
+      <c r="D33" t="s">
+        <v>238</v>
+      </c>
+      <c r="E33" t="s">
+        <v>239</v>
+      </c>
+      <c r="F33" t="s">
+        <v>239</v>
+      </c>
+      <c r="G33" t="s">
+        <v>239</v>
+      </c>
+      <c r="H33" t="s">
+        <v>239</v>
+      </c>
+      <c r="I33" t="s">
+        <v>239</v>
+      </c>
+      <c r="J33" t="s">
+        <v>239</v>
+      </c>
+      <c r="K33" t="s">
+        <v>239</v>
+      </c>
+      <c r="L33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>379</v>
+      </c>
+      <c r="C34" t="s">
+        <v>238</v>
+      </c>
+      <c r="D34" t="s">
+        <v>239</v>
+      </c>
+      <c r="E34" t="s">
+        <v>237</v>
+      </c>
+      <c r="G34" t="s">
+        <v>238</v>
+      </c>
+      <c r="H34" t="s">
+        <v>239</v>
+      </c>
+      <c r="I34" t="s">
+        <v>239</v>
+      </c>
+      <c r="J34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35" t="s">
+        <v>239</v>
+      </c>
+      <c r="C35" t="s">
+        <v>239</v>
+      </c>
+      <c r="D35" t="s">
+        <v>239</v>
+      </c>
+      <c r="E35" t="s">
+        <v>239</v>
+      </c>
+      <c r="F35" t="s">
+        <v>239</v>
+      </c>
+      <c r="G35" t="s">
+        <v>239</v>
+      </c>
+      <c r="H35" t="s">
+        <v>239</v>
+      </c>
+      <c r="I35" t="s">
+        <v>239</v>
+      </c>
+      <c r="J35" t="s">
+        <v>239</v>
+      </c>
+      <c r="K35" t="s">
+        <v>239</v>
+      </c>
+      <c r="L35" t="s">
+        <v>239</v>
+      </c>
+      <c r="M35" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>188</v>
+      </c>
+      <c r="F36" t="s">
+        <v>238</v>
+      </c>
+      <c r="G36" t="s">
+        <v>239</v>
+      </c>
+      <c r="H36" t="s">
+        <v>239</v>
+      </c>
+      <c r="I36" t="s">
+        <v>239</v>
+      </c>
+      <c r="J36" t="s">
+        <v>239</v>
+      </c>
+      <c r="K36" t="s">
+        <v>239</v>
+      </c>
+      <c r="L36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>239</v>
+      </c>
+      <c r="C37" t="s">
+        <v>239</v>
+      </c>
+      <c r="D37" t="s">
+        <v>239</v>
+      </c>
+      <c r="E37" t="s">
+        <v>239</v>
+      </c>
+      <c r="F37" t="s">
+        <v>239</v>
+      </c>
+      <c r="G37" t="s">
+        <v>239</v>
+      </c>
+      <c r="H37" t="s">
+        <v>239</v>
+      </c>
+      <c r="I37" t="s">
+        <v>239</v>
+      </c>
+      <c r="J37" t="s">
+        <v>239</v>
+      </c>
+      <c r="K37" t="s">
+        <v>239</v>
+      </c>
+      <c r="L37" t="s">
+        <v>239</v>
+      </c>
+      <c r="M37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C38" t="s">
+        <v>239</v>
+      </c>
+      <c r="D38" t="s">
+        <v>239</v>
+      </c>
+      <c r="E38" t="s">
+        <v>239</v>
+      </c>
+      <c r="F38" t="s">
+        <v>239</v>
+      </c>
+      <c r="G38" t="s">
+        <v>239</v>
+      </c>
+      <c r="H38" t="s">
+        <v>239</v>
+      </c>
+      <c r="I38" t="s">
+        <v>239</v>
+      </c>
+      <c r="J38" t="s">
+        <v>239</v>
+      </c>
+      <c r="K38" t="s">
+        <v>239</v>
+      </c>
+      <c r="L38" t="s">
+        <v>239</v>
+      </c>
+      <c r="M38" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>206</v>
+      </c>
+      <c r="B39" t="s">
+        <v>239</v>
+      </c>
+      <c r="C39" t="s">
+        <v>239</v>
+      </c>
+      <c r="D39" t="s">
+        <v>239</v>
+      </c>
+      <c r="E39" t="s">
+        <v>239</v>
+      </c>
+      <c r="F39" t="s">
+        <v>239</v>
+      </c>
+      <c r="G39" t="s">
+        <v>239</v>
+      </c>
+      <c r="H39" t="s">
+        <v>239</v>
+      </c>
+      <c r="I39" t="s">
+        <v>239</v>
+      </c>
+      <c r="J39" t="s">
+        <v>239</v>
+      </c>
+      <c r="K39" t="s">
+        <v>239</v>
+      </c>
+      <c r="L39" t="s">
+        <v>239</v>
+      </c>
+      <c r="M39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>373</v>
+      </c>
+      <c r="D40" t="s">
+        <v>238</v>
+      </c>
+      <c r="E40" t="s">
+        <v>239</v>
+      </c>
+      <c r="F40" t="s">
+        <v>239</v>
+      </c>
+      <c r="G40" t="s">
+        <v>239</v>
+      </c>
+      <c r="H40" t="s">
+        <v>239</v>
+      </c>
+      <c r="I40" t="s">
+        <v>239</v>
+      </c>
+      <c r="J40" t="s">
+        <v>239</v>
+      </c>
+      <c r="K40" t="s">
+        <v>239</v>
+      </c>
+      <c r="L40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41" t="s">
+        <v>238</v>
+      </c>
+      <c r="H41" t="s">
+        <v>239</v>
+      </c>
+      <c r="I41" t="s">
+        <v>239</v>
+      </c>
+      <c r="J41" t="s">
+        <v>239</v>
+      </c>
+      <c r="K41" t="s">
+        <v>239</v>
+      </c>
+      <c r="L41" t="s">
+        <v>239</v>
+      </c>
+      <c r="M41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>239</v>
+      </c>
+      <c r="C42" t="s">
+        <v>239</v>
+      </c>
+      <c r="D42" t="s">
+        <v>239</v>
+      </c>
+      <c r="E42" t="s">
+        <v>239</v>
+      </c>
+      <c r="F42" t="s">
+        <v>237</v>
+      </c>
+      <c r="L42" t="s">
+        <v>238</v>
+      </c>
+      <c r="M42" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>374</v>
+      </c>
+      <c r="C43" t="s">
+        <v>238</v>
+      </c>
+      <c r="D43" t="s">
+        <v>239</v>
+      </c>
+      <c r="E43" t="s">
+        <v>239</v>
+      </c>
+      <c r="F43" t="s">
+        <v>239</v>
+      </c>
+      <c r="G43" t="s">
+        <v>239</v>
+      </c>
+      <c r="H43" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" t="s">
+        <v>239</v>
+      </c>
+      <c r="C44" t="s">
+        <v>239</v>
+      </c>
+      <c r="D44" t="s">
+        <v>237</v>
+      </c>
+      <c r="M44" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>375</v>
+      </c>
+      <c r="B45" t="s">
+        <v>239</v>
+      </c>
+      <c r="C45" t="s">
+        <v>239</v>
+      </c>
+      <c r="D45" t="s">
+        <v>239</v>
+      </c>
+      <c r="E45" t="s">
+        <v>237</v>
+      </c>
+      <c r="K45" t="s">
+        <v>238</v>
+      </c>
+      <c r="L45" t="s">
+        <v>239</v>
+      </c>
+      <c r="M45" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>376</v>
+      </c>
+      <c r="B46" t="s">
+        <v>239</v>
+      </c>
+      <c r="C46" t="s">
+        <v>239</v>
+      </c>
+      <c r="D46" t="s">
+        <v>239</v>
+      </c>
+      <c r="E46" t="s">
+        <v>239</v>
+      </c>
+      <c r="F46" t="s">
+        <v>239</v>
+      </c>
+      <c r="G46" t="s">
+        <v>237</v>
+      </c>
+      <c r="M46" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>377</v>
+      </c>
+      <c r="D47" t="s">
+        <v>238</v>
+      </c>
+      <c r="E47" t="s">
+        <v>239</v>
+      </c>
+      <c r="F47" t="s">
+        <v>239</v>
+      </c>
+      <c r="G47" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>378</v>
+      </c>
+      <c r="B48" t="s">
+        <v>239</v>
+      </c>
+      <c r="C48" t="s">
+        <v>237</v>
+      </c>
+      <c r="L48" t="s">
+        <v>238</v>
+      </c>
+      <c r="M48" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F671E-F179-4448-8BD7-31034E28E8E3}">
+  <dimension ref="B1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787C0560-B6AC-43B7-9D40-0BAAE1936FD6}">
+  <dimension ref="B1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2613B65B-C97D-4F7F-A93B-55F0E2809563}">
+  <dimension ref="A1:M62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H3" t="s">
+        <v>239</v>
+      </c>
+      <c r="I3" t="s">
+        <v>239</v>
+      </c>
+      <c r="J3" t="s">
+        <v>239</v>
+      </c>
+      <c r="K3" t="s">
+        <v>239</v>
+      </c>
+      <c r="L3" t="s">
+        <v>239</v>
+      </c>
+      <c r="M3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" t="s">
+        <v>239</v>
+      </c>
+      <c r="I4" t="s">
+        <v>239</v>
+      </c>
+      <c r="J4" t="s">
+        <v>239</v>
+      </c>
+      <c r="K4" t="s">
+        <v>239</v>
+      </c>
+      <c r="L4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" t="s">
+        <v>239</v>
+      </c>
+      <c r="J5" t="s">
+        <v>239</v>
+      </c>
+      <c r="K5" t="s">
+        <v>239</v>
+      </c>
+      <c r="L5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E6" t="s">
+        <v>239</v>
+      </c>
+      <c r="J6" t="s">
+        <v>239</v>
+      </c>
+      <c r="K6" t="s">
+        <v>239</v>
+      </c>
+      <c r="L6" t="s">
+        <v>239</v>
+      </c>
+      <c r="M6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F7" t="s">
+        <v>239</v>
+      </c>
+      <c r="G7" t="s">
+        <v>239</v>
+      </c>
+      <c r="J7" t="s">
+        <v>239</v>
+      </c>
+      <c r="K7" t="s">
+        <v>239</v>
+      </c>
+      <c r="L7" t="s">
+        <v>239</v>
+      </c>
+      <c r="M7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E8" t="s">
+        <v>239</v>
+      </c>
+      <c r="F8" t="s">
+        <v>239</v>
+      </c>
+      <c r="G8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I8" t="s">
+        <v>239</v>
+      </c>
+      <c r="J8" t="s">
+        <v>239</v>
+      </c>
+      <c r="K8" t="s">
+        <v>239</v>
+      </c>
+      <c r="L8" t="s">
+        <v>239</v>
+      </c>
+      <c r="M8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>239</v>
+      </c>
+      <c r="K9" t="s">
+        <v>239</v>
+      </c>
+      <c r="L9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" t="s">
+        <v>239</v>
+      </c>
+      <c r="E10" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" t="s">
+        <v>239</v>
+      </c>
+      <c r="G10" t="s">
+        <v>239</v>
+      </c>
+      <c r="H10" t="s">
+        <v>239</v>
+      </c>
+      <c r="I10" t="s">
+        <v>239</v>
+      </c>
+      <c r="J10" t="s">
+        <v>239</v>
+      </c>
+      <c r="K10" t="s">
+        <v>239</v>
+      </c>
+      <c r="L10" t="s">
+        <v>239</v>
+      </c>
+      <c r="M10" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" t="s">
+        <v>239</v>
+      </c>
+      <c r="E11" t="s">
+        <v>239</v>
+      </c>
+      <c r="F11" t="s">
+        <v>239</v>
+      </c>
+      <c r="G11" t="s">
+        <v>239</v>
+      </c>
+      <c r="J11" t="s">
+        <v>239</v>
+      </c>
+      <c r="K11" t="s">
+        <v>239</v>
+      </c>
+      <c r="L11" t="s">
+        <v>239</v>
+      </c>
+      <c r="M11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
+        <v>239</v>
+      </c>
+      <c r="I12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>239</v>
+      </c>
+      <c r="I13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>239</v>
+      </c>
+      <c r="I14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" t="s">
+        <v>239</v>
+      </c>
+      <c r="G15" t="s">
+        <v>239</v>
+      </c>
+      <c r="H15" t="s">
+        <v>239</v>
+      </c>
+      <c r="I15" t="s">
+        <v>239</v>
+      </c>
+      <c r="J15" t="s">
+        <v>239</v>
+      </c>
+      <c r="K15" t="s">
+        <v>239</v>
+      </c>
+      <c r="L15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>272</v>
+      </c>
+      <c r="J16" t="s">
+        <v>239</v>
+      </c>
+      <c r="K16" t="s">
+        <v>239</v>
+      </c>
+      <c r="L16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" t="s">
+        <v>239</v>
+      </c>
+      <c r="I17" t="s">
+        <v>239</v>
+      </c>
+      <c r="J17" t="s">
+        <v>239</v>
+      </c>
+      <c r="K17" t="s">
+        <v>239</v>
+      </c>
+      <c r="L17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C18" t="s">
+        <v>239</v>
+      </c>
+      <c r="D18" t="s">
+        <v>239</v>
+      </c>
+      <c r="E18" t="s">
+        <v>239</v>
+      </c>
+      <c r="F18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G18" t="s">
+        <v>239</v>
+      </c>
+      <c r="J18" t="s">
+        <v>239</v>
+      </c>
+      <c r="K18" t="s">
+        <v>239</v>
+      </c>
+      <c r="L18" t="s">
+        <v>239</v>
+      </c>
+      <c r="M18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19" t="s">
+        <v>239</v>
+      </c>
+      <c r="D19" t="s">
+        <v>239</v>
+      </c>
+      <c r="E19" t="s">
+        <v>239</v>
+      </c>
+      <c r="M19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>239</v>
+      </c>
+      <c r="G20" t="s">
+        <v>239</v>
+      </c>
+      <c r="J20" t="s">
+        <v>239</v>
+      </c>
+      <c r="K20" t="s">
+        <v>239</v>
+      </c>
+      <c r="L20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" t="s">
+        <v>239</v>
+      </c>
+      <c r="G21" t="s">
+        <v>239</v>
+      </c>
+      <c r="J21" t="s">
+        <v>239</v>
+      </c>
+      <c r="K21" t="s">
+        <v>239</v>
+      </c>
+      <c r="L21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" t="s">
+        <v>239</v>
+      </c>
+      <c r="I22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>239</v>
+      </c>
+      <c r="C23" t="s">
+        <v>239</v>
+      </c>
+      <c r="D23" t="s">
+        <v>239</v>
+      </c>
+      <c r="E23" t="s">
+        <v>239</v>
+      </c>
+      <c r="F23" t="s">
+        <v>239</v>
+      </c>
+      <c r="G23" t="s">
+        <v>239</v>
+      </c>
+      <c r="J23" t="s">
+        <v>239</v>
+      </c>
+      <c r="K23" t="s">
+        <v>239</v>
+      </c>
+      <c r="L23" t="s">
+        <v>239</v>
+      </c>
+      <c r="M23" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" t="s">
+        <v>239</v>
+      </c>
+      <c r="D24" t="s">
+        <v>239</v>
+      </c>
+      <c r="E24" t="s">
+        <v>239</v>
+      </c>
+      <c r="J24" t="s">
+        <v>239</v>
+      </c>
+      <c r="K24" t="s">
+        <v>239</v>
+      </c>
+      <c r="L24" t="s">
+        <v>239</v>
+      </c>
+      <c r="M24" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" t="s">
+        <v>239</v>
+      </c>
+      <c r="G25" t="s">
+        <v>239</v>
+      </c>
+      <c r="J25" t="s">
+        <v>239</v>
+      </c>
+      <c r="K25" t="s">
+        <v>239</v>
+      </c>
+      <c r="L25" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>239</v>
+      </c>
+      <c r="C26" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26" t="s">
+        <v>239</v>
+      </c>
+      <c r="E26" t="s">
+        <v>239</v>
+      </c>
+      <c r="J26" t="s">
+        <v>239</v>
+      </c>
+      <c r="K26" t="s">
+        <v>239</v>
+      </c>
+      <c r="L26" t="s">
+        <v>239</v>
+      </c>
+      <c r="M26" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" t="s">
+        <v>239</v>
+      </c>
+      <c r="G27" t="s">
+        <v>239</v>
+      </c>
+      <c r="J27" t="s">
+        <v>239</v>
+      </c>
+      <c r="K27" t="s">
+        <v>239</v>
+      </c>
+      <c r="L27" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" t="s">
+        <v>239</v>
+      </c>
+      <c r="G28" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" t="s">
+        <v>239</v>
+      </c>
+      <c r="C29" t="s">
+        <v>239</v>
+      </c>
+      <c r="D29" t="s">
+        <v>239</v>
+      </c>
+      <c r="E29" t="s">
+        <v>239</v>
+      </c>
+      <c r="J29" t="s">
+        <v>239</v>
+      </c>
+      <c r="K29" t="s">
+        <v>239</v>
+      </c>
+      <c r="L29" t="s">
+        <v>239</v>
+      </c>
+      <c r="M29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" t="s">
+        <v>239</v>
+      </c>
+      <c r="G30" t="s">
+        <v>239</v>
+      </c>
+      <c r="J30" t="s">
+        <v>239</v>
+      </c>
+      <c r="K30" t="s">
+        <v>239</v>
+      </c>
+      <c r="L30" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>161</v>
+      </c>
+      <c r="H31" t="s">
+        <v>239</v>
+      </c>
+      <c r="I31" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>239</v>
+      </c>
+      <c r="C32" t="s">
+        <v>239</v>
+      </c>
+      <c r="D32" t="s">
+        <v>239</v>
+      </c>
+      <c r="E32" t="s">
+        <v>239</v>
+      </c>
+      <c r="J32" t="s">
+        <v>239</v>
+      </c>
+      <c r="K32" t="s">
+        <v>239</v>
+      </c>
+      <c r="L32" t="s">
+        <v>239</v>
+      </c>
+      <c r="M32" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
+        <v>239</v>
+      </c>
+      <c r="C33" t="s">
+        <v>239</v>
+      </c>
+      <c r="D33" t="s">
+        <v>239</v>
+      </c>
+      <c r="E33" t="s">
+        <v>239</v>
+      </c>
+      <c r="F33" t="s">
+        <v>239</v>
+      </c>
+      <c r="G33" t="s">
+        <v>239</v>
+      </c>
+      <c r="J33" t="s">
+        <v>239</v>
+      </c>
+      <c r="K33" t="s">
+        <v>239</v>
+      </c>
+      <c r="L33" t="s">
+        <v>239</v>
+      </c>
+      <c r="M33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>154</v>
+      </c>
+      <c r="H34" t="s">
+        <v>239</v>
+      </c>
+      <c r="I34" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" t="s">
+        <v>239</v>
+      </c>
+      <c r="I35" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>239</v>
+      </c>
+      <c r="C36" t="s">
+        <v>239</v>
+      </c>
+      <c r="D36" t="s">
+        <v>239</v>
+      </c>
+      <c r="E36" t="s">
+        <v>239</v>
+      </c>
+      <c r="F36" t="s">
+        <v>239</v>
+      </c>
+      <c r="G36" t="s">
+        <v>239</v>
+      </c>
+      <c r="J36" t="s">
+        <v>239</v>
+      </c>
+      <c r="K36" t="s">
+        <v>239</v>
+      </c>
+      <c r="L36" t="s">
+        <v>239</v>
+      </c>
+      <c r="M36" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>239</v>
+      </c>
+      <c r="C37" t="s">
+        <v>239</v>
+      </c>
+      <c r="D37" t="s">
+        <v>239</v>
+      </c>
+      <c r="E37" t="s">
+        <v>239</v>
+      </c>
+      <c r="J37" t="s">
+        <v>239</v>
+      </c>
+      <c r="K37" t="s">
+        <v>239</v>
+      </c>
+      <c r="L37" t="s">
+        <v>239</v>
+      </c>
+      <c r="M37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="H38" t="s">
+        <v>239</v>
+      </c>
+      <c r="I38" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" t="s">
+        <v>239</v>
+      </c>
+      <c r="C39" t="s">
+        <v>239</v>
+      </c>
+      <c r="D39" t="s">
+        <v>239</v>
+      </c>
+      <c r="E39" t="s">
+        <v>239</v>
+      </c>
+      <c r="F39" t="s">
+        <v>239</v>
+      </c>
+      <c r="G39" t="s">
+        <v>239</v>
+      </c>
+      <c r="H39" t="s">
+        <v>239</v>
+      </c>
+      <c r="I39" t="s">
+        <v>239</v>
+      </c>
+      <c r="J39" t="s">
+        <v>239</v>
+      </c>
+      <c r="K39" t="s">
+        <v>239</v>
+      </c>
+      <c r="L39" t="s">
+        <v>239</v>
+      </c>
+      <c r="M39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" t="s">
+        <v>239</v>
+      </c>
+      <c r="G40" t="s">
+        <v>239</v>
+      </c>
+      <c r="H40" t="s">
+        <v>239</v>
+      </c>
+      <c r="I40" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
+        <v>239</v>
+      </c>
+      <c r="C41" t="s">
+        <v>239</v>
+      </c>
+      <c r="D41" t="s">
+        <v>239</v>
+      </c>
+      <c r="E41" t="s">
+        <v>239</v>
+      </c>
+      <c r="F41" t="s">
+        <v>239</v>
+      </c>
+      <c r="G41" t="s">
+        <v>239</v>
+      </c>
+      <c r="H41" t="s">
+        <v>239</v>
+      </c>
+      <c r="I41" t="s">
+        <v>239</v>
+      </c>
+      <c r="M41" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>252</v>
+      </c>
+      <c r="B42" t="s">
+        <v>239</v>
+      </c>
+      <c r="C42" t="s">
+        <v>239</v>
+      </c>
+      <c r="D42" t="s">
+        <v>239</v>
+      </c>
+      <c r="E42" t="s">
+        <v>239</v>
+      </c>
+      <c r="F42" t="s">
+        <v>239</v>
+      </c>
+      <c r="G42" t="s">
+        <v>239</v>
+      </c>
+      <c r="H42" t="s">
+        <v>239</v>
+      </c>
+      <c r="I42" t="s">
+        <v>239</v>
+      </c>
+      <c r="J42" t="s">
+        <v>239</v>
+      </c>
+      <c r="K42" t="s">
+        <v>239</v>
+      </c>
+      <c r="L42" t="s">
+        <v>239</v>
+      </c>
+      <c r="M42" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43" t="s">
+        <v>239</v>
+      </c>
+      <c r="I43" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" t="s">
+        <v>239</v>
+      </c>
+      <c r="I44" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>136</v>
+      </c>
+      <c r="H45" t="s">
+        <v>239</v>
+      </c>
+      <c r="I45" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" t="s">
+        <v>239</v>
+      </c>
+      <c r="I46" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>268</v>
+      </c>
+      <c r="J47" t="s">
+        <v>239</v>
+      </c>
+      <c r="K47" t="s">
+        <v>239</v>
+      </c>
+      <c r="L47" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="J48" t="s">
+        <v>239</v>
+      </c>
+      <c r="K48" t="s">
+        <v>239</v>
+      </c>
+      <c r="L48" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" t="s">
+        <v>239</v>
+      </c>
+      <c r="C49" t="s">
+        <v>239</v>
+      </c>
+      <c r="D49" t="s">
+        <v>239</v>
+      </c>
+      <c r="E49" t="s">
+        <v>239</v>
+      </c>
+      <c r="M49" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>380</v>
+      </c>
+      <c r="H50" t="s">
+        <v>239</v>
+      </c>
+      <c r="I50" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>253</v>
+      </c>
+      <c r="B51" t="s">
+        <v>239</v>
+      </c>
+      <c r="C51" t="s">
+        <v>239</v>
+      </c>
+      <c r="D51" t="s">
+        <v>239</v>
+      </c>
+      <c r="E51" t="s">
+        <v>239</v>
+      </c>
+      <c r="F51" t="s">
+        <v>239</v>
+      </c>
+      <c r="G51" t="s">
+        <v>239</v>
+      </c>
+      <c r="J51" t="s">
+        <v>239</v>
+      </c>
+      <c r="K51" t="s">
+        <v>239</v>
+      </c>
+      <c r="L51" t="s">
+        <v>239</v>
+      </c>
+      <c r="M51" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" t="s">
+        <v>239</v>
+      </c>
+      <c r="C52" t="s">
+        <v>239</v>
+      </c>
+      <c r="D52" t="s">
+        <v>239</v>
+      </c>
+      <c r="E52" t="s">
+        <v>239</v>
+      </c>
+      <c r="F52" t="s">
+        <v>239</v>
+      </c>
+      <c r="G52" t="s">
+        <v>239</v>
+      </c>
+      <c r="H52" t="s">
+        <v>239</v>
+      </c>
+      <c r="I52" t="s">
+        <v>239</v>
+      </c>
+      <c r="J52" t="s">
+        <v>239</v>
+      </c>
+      <c r="K52" t="s">
+        <v>239</v>
+      </c>
+      <c r="L52" t="s">
+        <v>239</v>
+      </c>
+      <c r="M52" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>381</v>
+      </c>
+      <c r="B53" t="s">
+        <v>239</v>
+      </c>
+      <c r="C53" t="s">
+        <v>239</v>
+      </c>
+      <c r="D53" t="s">
+        <v>239</v>
+      </c>
+      <c r="E53" t="s">
+        <v>239</v>
+      </c>
+      <c r="F53" t="s">
+        <v>239</v>
+      </c>
+      <c r="G53" t="s">
+        <v>239</v>
+      </c>
+      <c r="H53" t="s">
+        <v>239</v>
+      </c>
+      <c r="I53" t="s">
+        <v>239</v>
+      </c>
+      <c r="J53" t="s">
+        <v>239</v>
+      </c>
+      <c r="K53" t="s">
+        <v>239</v>
+      </c>
+      <c r="L53" t="s">
+        <v>239</v>
+      </c>
+      <c r="M53" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>254</v>
+      </c>
+      <c r="H54" t="s">
+        <v>239</v>
+      </c>
+      <c r="I54" t="s">
+        <v>239</v>
+      </c>
+      <c r="J54" t="s">
+        <v>239</v>
+      </c>
+      <c r="K54" t="s">
+        <v>239</v>
+      </c>
+      <c r="L54" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" t="s">
+        <v>239</v>
+      </c>
+      <c r="C55" t="s">
+        <v>239</v>
+      </c>
+      <c r="D55" t="s">
+        <v>239</v>
+      </c>
+      <c r="E55" t="s">
+        <v>239</v>
+      </c>
+      <c r="M55" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" t="s">
+        <v>239</v>
+      </c>
+      <c r="I56" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" t="s">
+        <v>239</v>
+      </c>
+      <c r="C57" t="s">
+        <v>239</v>
+      </c>
+      <c r="D57" t="s">
+        <v>239</v>
+      </c>
+      <c r="E57" t="s">
+        <v>239</v>
+      </c>
+      <c r="F57" t="s">
+        <v>239</v>
+      </c>
+      <c r="G57" t="s">
+        <v>239</v>
+      </c>
+      <c r="J57" t="s">
+        <v>239</v>
+      </c>
+      <c r="K57" t="s">
+        <v>239</v>
+      </c>
+      <c r="L57" t="s">
+        <v>239</v>
+      </c>
+      <c r="M57" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>382</v>
+      </c>
+      <c r="B58" t="s">
+        <v>239</v>
+      </c>
+      <c r="C58" t="s">
+        <v>239</v>
+      </c>
+      <c r="D58" t="s">
+        <v>239</v>
+      </c>
+      <c r="E58" t="s">
+        <v>239</v>
+      </c>
+      <c r="J58" t="s">
+        <v>239</v>
+      </c>
+      <c r="K58" t="s">
+        <v>239</v>
+      </c>
+      <c r="L58" t="s">
+        <v>239</v>
+      </c>
+      <c r="M58" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>65</v>
+      </c>
+      <c r="H59" t="s">
+        <v>239</v>
+      </c>
+      <c r="I59" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>47</v>
+      </c>
+      <c r="H60" t="s">
+        <v>239</v>
+      </c>
+      <c r="I60" t="s">
+        <v>239</v>
+      </c>
+      <c r="J60" t="s">
+        <v>239</v>
+      </c>
+      <c r="K60" t="s">
+        <v>239</v>
+      </c>
+      <c r="L60" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" t="s">
+        <v>239</v>
+      </c>
+      <c r="G61" t="s">
+        <v>239</v>
+      </c>
+      <c r="H61" t="s">
+        <v>239</v>
+      </c>
+      <c r="I61" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>127</v>
+      </c>
+      <c r="H62" t="s">
+        <v>239</v>
+      </c>
+      <c r="I62" t="s">
         <v>239</v>
       </c>
     </row>

</xml_diff>